<commit_message>
Opsplitsen per subset ingebouwd.
TODO: Significantie tegenover een totaal van een subset toevoegen.
</commit_message>
<xml_diff>
--- a/configuratie.xlsx
+++ b/configuratie.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ggdnog-my.sharepoint.com/personal/a_dijkstra_ggdnog_nl/Documents/Documenten/Tabellenboek/GGData_tabellenboek/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="43" documentId="8_{0F18ABD2-A895-4412-9B00-D736EAC011EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6E6148BD-37BB-4611-A8B0-A4C4617C42A8}"/>
+  <xr:revisionPtr revIDLastSave="53" documentId="8_{0F18ABD2-A895-4412-9B00-D736EAC011EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3E3EC7E8-44C8-4CC4-9C82-57CB9D10ACDE}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="78">
   <si>
     <t>naam_dataset</t>
   </si>
@@ -268,6 +268,12 @@
   </si>
   <si>
     <t>jaar</t>
+  </si>
+  <si>
+    <t>Gemeentecode</t>
+  </si>
+  <si>
+    <t>subregio</t>
   </si>
 </sst>
 </file>
@@ -727,7 +733,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -735,8 +741,8 @@
     <col min="1" max="1" width="17.5703125" customWidth="1"/>
     <col min="2" max="2" width="38.7109375" customWidth="1"/>
     <col min="3" max="3" width="15.140625" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -826,7 +832,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C74130A8-7C80-4EF0-924A-78FEEA1CDE59}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
@@ -835,7 +841,8 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="3" width="17.28515625" customWidth="1"/>
+    <col min="2" max="2" width="21" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
     <col min="4" max="4" width="14.28515625" customWidth="1"/>
     <col min="5" max="5" width="13.85546875" customWidth="1"/>
   </cols>
@@ -864,6 +871,9 @@
       <c r="A2" t="s">
         <v>6</v>
       </c>
+      <c r="B2" t="s">
+        <v>76</v>
+      </c>
       <c r="C2">
         <v>2022</v>
       </c>
@@ -879,10 +889,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>77</v>
       </c>
       <c r="C3">
-        <v>2019</v>
+        <v>2022</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>
@@ -890,12 +903,26 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4">
+        <v>2019</v>
+      </c>
+      <c r="D4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="C4">
+      <c r="C5">
         <v>2022</v>
       </c>
-      <c r="D4" t="b">
+      <c r="D5" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Verdere uitwerking van output naar Excel.
</commit_message>
<xml_diff>
--- a/configuratie.xlsx
+++ b/configuratie.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ggdnog-my.sharepoint.com/personal/a_dijkstra_ggdnog_nl/Documents/Documenten/Tabellenboek/GGData_tabellenboek/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="53" documentId="8_{0F18ABD2-A895-4412-9B00-D736EAC011EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3E3EC7E8-44C8-4CC4-9C82-57CB9D10ACDE}"/>
+  <xr:revisionPtr revIDLastSave="69" documentId="8_{0F18ABD2-A895-4412-9B00-D736EAC011EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8337355B-C053-443C-A02E-EA0DFB2DD377}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
   </bookViews>
   <sheets>
     <sheet name="algemeen" sheetId="5" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="onderdelen" sheetId="4" r:id="rId3"/>
     <sheet name="indeling_rijen" sheetId="2" r:id="rId4"/>
     <sheet name="crossings" sheetId="3" r:id="rId5"/>
+    <sheet name="opmaak" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="105">
   <si>
     <t>naam_dataset</t>
   </si>
@@ -207,9 +208,6 @@
     <t>../../Script tabellenboek/data/Totaalbestand cGM JV 2022.sav</t>
   </si>
   <si>
-    <t>bestaande_csv_opnieuw_berekenen</t>
-  </si>
-  <si>
     <t>min_observaties_per_vraag</t>
   </si>
   <si>
@@ -228,12 +226,6 @@
     <t>sign_toetsen</t>
   </si>
   <si>
-    <t>subsets_moeten_voorkomen_in_onderwerp_tbb</t>
-  </si>
-  <si>
-    <t>alleen_tbb_met_actuele_gegevens</t>
-  </si>
-  <si>
     <t>missing_weegfactoren</t>
   </si>
   <si>
@@ -274,6 +266,96 @@
   </si>
   <si>
     <t>subregio</t>
+  </si>
+  <si>
+    <t>waarde</t>
+  </si>
+  <si>
+    <t>#FFFFFF</t>
+  </si>
+  <si>
+    <t>bold</t>
+  </si>
+  <si>
+    <t>titel_fill</t>
+  </si>
+  <si>
+    <t>#D1005D</t>
+  </si>
+  <si>
+    <t>kop_fill</t>
+  </si>
+  <si>
+    <t>#1D1756</t>
+  </si>
+  <si>
+    <t>rij_hoogte</t>
+  </si>
+  <si>
+    <t>rij_hoogte_kop</t>
+  </si>
+  <si>
+    <t>kolombreedte_antwoorden</t>
+  </si>
+  <si>
+    <t>kolombreedte</t>
+  </si>
+  <si>
+    <t>font_color</t>
+  </si>
+  <si>
+    <t>#000000</t>
+  </si>
+  <si>
+    <t>font_type</t>
+  </si>
+  <si>
+    <t>Calibri</t>
+  </si>
+  <si>
+    <t>border_tussen_gegevens</t>
+  </si>
+  <si>
+    <t>rijen_afwisselend_kleuren</t>
+  </si>
+  <si>
+    <t>kolommen_afwisselend_kleuren</t>
+  </si>
+  <si>
+    <t>kolommen_crossings_kleuren</t>
+  </si>
+  <si>
+    <t>header_stijl</t>
+  </si>
+  <si>
+    <t>enkel</t>
+  </si>
+  <si>
+    <t>crossing_headers_kleiner</t>
+  </si>
+  <si>
+    <t>label_max_lengte</t>
+  </si>
+  <si>
+    <t>titel_decoration</t>
+  </si>
+  <si>
+    <t>titel_color</t>
+  </si>
+  <si>
+    <t>titel_size</t>
+  </si>
+  <si>
+    <t>kop_size</t>
+  </si>
+  <si>
+    <t>kop_color</t>
+  </si>
+  <si>
+    <t>kop_decoration</t>
+  </si>
+  <si>
+    <t>font_size</t>
   </si>
 </sst>
 </file>
@@ -625,23 +707,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB9555E0-3443-4710-AD14-3A977E907E6B}">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" customWidth="1"/>
-    <col min="10" max="10" width="11.5703125" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -670,56 +750,38 @@
         <v>63</v>
       </c>
       <c r="J1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>100</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
         <v>64</v>
       </c>
-      <c r="K1" t="s">
+      <c r="D2" t="s">
         <v>65</v>
       </c>
-      <c r="L1" t="s">
+      <c r="E2" t="s">
         <v>66</v>
       </c>
-      <c r="M1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" t="b">
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>100</v>
-      </c>
-      <c r="C2">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="H2">
+        <v>0.01</v>
+      </c>
+      <c r="I2" t="s">
         <v>67</v>
       </c>
-      <c r="E2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F2" t="s">
-        <v>69</v>
-      </c>
-      <c r="G2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H2" t="b">
-        <v>0</v>
-      </c>
-      <c r="I2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>0.99</v>
-      </c>
-      <c r="L2" t="s">
-        <v>70</v>
-      </c>
-      <c r="M2" t="b">
+      <c r="J2" t="b">
         <v>1</v>
       </c>
     </row>
@@ -832,10 +894,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C74130A8-7C80-4EF0-924A-78FEEA1CDE59}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -855,16 +917,16 @@
         <v>51</v>
       </c>
       <c r="C1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D1" t="s">
         <v>50</v>
       </c>
       <c r="E1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -872,7 +934,7 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C2">
         <v>2022</v>
@@ -881,7 +943,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
@@ -892,7 +954,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C3">
         <v>2022</v>
@@ -903,13 +965,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>76</v>
+        <v>6</v>
       </c>
       <c r="C4">
-        <v>2019</v>
+        <v>2022</v>
       </c>
       <c r="D4" t="b">
         <v>0</v>
@@ -917,12 +976,26 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5">
+        <v>2019</v>
+      </c>
+      <c r="D5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="C5">
+      <c r="C6">
         <v>2022</v>
       </c>
-      <c r="D5" t="b">
+      <c r="D6" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1172,4 +1245,207 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DD3CC7F-96FA-4722-9354-DA6065EED849}">
+  <dimension ref="A1:B23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.140625" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>103</v>
+      </c>
+      <c r="B8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>84</v>
+      </c>
+      <c r="B12">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>85</v>
+      </c>
+      <c r="B13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>86</v>
+      </c>
+      <c r="B14" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>88</v>
+      </c>
+      <c r="B15" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>104</v>
+      </c>
+      <c r="B16">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>90</v>
+      </c>
+      <c r="B17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>91</v>
+      </c>
+      <c r="B18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>92</v>
+      </c>
+      <c r="B19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>93</v>
+      </c>
+      <c r="B20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>94</v>
+      </c>
+      <c r="B21" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>96</v>
+      </c>
+      <c r="B22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>97</v>
+      </c>
+      <c r="B23">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Genereren van Excelsheets verder uitgewerkt.
</commit_message>
<xml_diff>
--- a/configuratie.xlsx
+++ b/configuratie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ggdnog-my.sharepoint.com/personal/a_dijkstra_ggdnog_nl/Documents/Documenten/Tabellenboek/GGData_tabellenboek/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="69" documentId="8_{0F18ABD2-A895-4412-9B00-D736EAC011EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8337355B-C053-443C-A02E-EA0DFB2DD377}"/>
+  <xr:revisionPtr revIDLastSave="73" documentId="8_{0F18ABD2-A895-4412-9B00-D736EAC011EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1C1087F5-E8D0-4452-A59E-E1BE55B8A231}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="105">
   <si>
     <t>naam_dataset</t>
   </si>
@@ -328,9 +328,6 @@
     <t>header_stijl</t>
   </si>
   <si>
-    <t>enkel</t>
-  </si>
-  <si>
     <t>crossing_headers_kleiner</t>
   </si>
   <si>
@@ -356,6 +353,9 @@
   </si>
   <si>
     <t>font_size</t>
+  </si>
+  <si>
+    <t>dubbel</t>
   </si>
 </sst>
 </file>
@@ -707,10 +707,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB9555E0-3443-4710-AD14-3A977E907E6B}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -721,7 +721,7 @@
     <col min="7" max="7" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -752,8 +752,11 @@
       <c r="J1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>100</v>
       </c>
@@ -783,6 +786,9 @@
       </c>
       <c r="J2" t="b">
         <v>1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -792,10 +798,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27E157EC-B8A8-4DD4-B0B0-EC0F5BEAABD9}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F1" sqref="F1:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -807,7 +813,7 @@
     <col min="5" max="5" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -823,11 +829,8 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -843,11 +846,8 @@
       <c r="E2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -863,11 +863,8 @@
       <c r="E3" t="s">
         <v>14</v>
       </c>
-      <c r="F3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -882,9 +879,6 @@
       </c>
       <c r="E4" t="s">
         <v>16</v>
-      </c>
-      <c r="F4" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -1251,8 +1245,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DD3CC7F-96FA-4722-9354-DA6065EED849}">
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1271,7 +1265,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B2">
         <v>14</v>
@@ -1279,7 +1273,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B3" t="s">
         <v>76</v>
@@ -1287,7 +1281,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B4" t="s">
         <v>77</v>
@@ -1303,7 +1297,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B6">
         <v>14</v>
@@ -1311,7 +1305,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B7" t="s">
         <v>76</v>
@@ -1319,7 +1313,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B8" t="s">
         <v>77</v>
@@ -1383,7 +1377,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B16">
         <v>11</v>
@@ -1426,12 +1420,12 @@
         <v>94</v>
       </c>
       <c r="B21" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B22" t="b">
         <v>1</v>
@@ -1439,7 +1433,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B23">
         <v>66</v>

</xml_diff>

<commit_message>
Exporteren zonder subset nu ook mogelijk. Verder opmerkingen Henk verwerkt en begin gemaakt met herschrijven van de handleiding.
</commit_message>
<xml_diff>
--- a/configuratie.xlsx
+++ b/configuratie.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ggdnog-my.sharepoint.com/personal/a_dijkstra_ggdnog_nl/Documents/Documenten/Tabellenboek/GGData_tabellenboek/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="73" documentId="8_{0F18ABD2-A895-4412-9B00-D736EAC011EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1C1087F5-E8D0-4452-A59E-E1BE55B8A231}"/>
+  <xr:revisionPtr revIDLastSave="99" documentId="8_{0F18ABD2-A895-4412-9B00-D736EAC011EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2FB37809-533C-4437-B63A-5BC439FE9669}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
   </bookViews>
   <sheets>
     <sheet name="algemeen" sheetId="5" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="indeling_rijen" sheetId="2" r:id="rId4"/>
     <sheet name="crossings" sheetId="3" r:id="rId5"/>
     <sheet name="opmaak" sheetId="6" r:id="rId6"/>
+    <sheet name="labelcorrectie" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="116">
   <si>
     <t>naam_dataset</t>
   </si>
@@ -356,6 +357,39 @@
   </si>
   <si>
     <t>dubbel</t>
+  </si>
+  <si>
+    <t>header_template</t>
+  </si>
+  <si>
+    <t>Totaal [naam] [jaar]</t>
+  </si>
+  <si>
+    <t>var_label</t>
+  </si>
+  <si>
+    <t>antwoord_waarde</t>
+  </si>
+  <si>
+    <t>antwoord_oud</t>
+  </si>
+  <si>
+    <t>antwoord_nieuw</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Abc</t>
+  </si>
+  <si>
+    <t>Alleen opleiding</t>
+  </si>
+  <si>
+    <t>Werkt, volgt geen opleiding</t>
+  </si>
+  <si>
+    <t>Geen opleiding</t>
   </si>
 </sst>
 </file>
@@ -371,12 +405,17 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -391,8 +430,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -1243,10 +1285,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DD3CC7F-96FA-4722-9354-DA6065EED849}">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1425,18 +1467,98 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>95</v>
-      </c>
-      <c r="B22" t="b">
-        <v>1</v>
+        <v>105</v>
+      </c>
+      <c r="B22" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>95</v>
+      </c>
+      <c r="B23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>96</v>
       </c>
-      <c r="B23">
+      <c r="B24">
         <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B22162FB-19FC-4D35-A378-DB18D18AE0D2}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="2" max="2" width="21" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" t="s">
+        <v>114</v>
+      </c>
+      <c r="E4" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mogelijkheid voor andere weegfactoren per variabele ingebouwd. Verder een aantal kleine onderdelen toegevoegd van het vorige script: - introtekst - logo's
</commit_message>
<xml_diff>
--- a/configuratie.xlsx
+++ b/configuratie.xlsx
@@ -8,18 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ggdnog-my.sharepoint.com/personal/a_dijkstra_ggdnog_nl/Documents/Documenten/Tabellenboek/GGData_tabellenboek/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="99" documentId="8_{0F18ABD2-A895-4412-9B00-D736EAC011EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2FB37809-533C-4437-B63A-5BC439FE9669}"/>
+  <xr:revisionPtr revIDLastSave="136" documentId="8_{0F18ABD2-A895-4412-9B00-D736EAC011EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FAAC9A4E-7792-45BF-AD6C-4E5507B8555D}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
   </bookViews>
   <sheets>
     <sheet name="algemeen" sheetId="5" r:id="rId1"/>
-    <sheet name="datasets" sheetId="1" r:id="rId2"/>
-    <sheet name="onderdelen" sheetId="4" r:id="rId3"/>
-    <sheet name="indeling_rijen" sheetId="2" r:id="rId4"/>
-    <sheet name="crossings" sheetId="3" r:id="rId5"/>
-    <sheet name="opmaak" sheetId="6" r:id="rId6"/>
+    <sheet name="crossings" sheetId="3" r:id="rId2"/>
+    <sheet name="headers_afkortingen" sheetId="10" r:id="rId3"/>
+    <sheet name="datasets" sheetId="1" r:id="rId4"/>
+    <sheet name="indeling_rijen" sheetId="2" r:id="rId5"/>
+    <sheet name="intro_tekst" sheetId="9" r:id="rId6"/>
     <sheet name="labelcorrectie" sheetId="7" r:id="rId7"/>
+    <sheet name="logos" sheetId="8" r:id="rId8"/>
+    <sheet name="onderdelen" sheetId="4" r:id="rId9"/>
+    <sheet name="opmaak" sheetId="6" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="130">
   <si>
     <t>naam_dataset</t>
   </si>
@@ -233,9 +236,6 @@
     <t>confidence_level</t>
   </si>
   <si>
-    <t>weergave_type</t>
-  </si>
-  <si>
     <t>*</t>
   </si>
   <si>
@@ -245,9 +245,6 @@
     <t>-</t>
   </si>
   <si>
-    <t>percentage</t>
-  </si>
-  <si>
     <t>multithreading</t>
   </si>
   <si>
@@ -390,6 +387,54 @@
   </si>
   <si>
     <t>Geen opleiding</t>
+  </si>
+  <si>
+    <t>bestand</t>
+  </si>
+  <si>
+    <t>rij</t>
+  </si>
+  <si>
+    <t>kolom</t>
+  </si>
+  <si>
+    <t>breedte</t>
+  </si>
+  <si>
+    <t>hoogte</t>
+  </si>
+  <si>
+    <t>Tabellenboek [naam]</t>
+  </si>
+  <si>
+    <t>tekst</t>
+  </si>
+  <si>
+    <t>Dit tabellenboek is een conceptversie.</t>
+  </si>
+  <si>
+    <t>Iedere GGD kan dit tabellenboek zelf uitdraaien met een specifieke configuratie.</t>
+  </si>
+  <si>
+    <t>vervanging</t>
+  </si>
+  <si>
+    <t>Achterhoek</t>
+  </si>
+  <si>
+    <t>AH</t>
+  </si>
+  <si>
+    <t>Noord-Veluwe</t>
+  </si>
+  <si>
+    <t>N-V</t>
+  </si>
+  <si>
+    <t>Midden-IJssel Oost-Veluwe</t>
+  </si>
+  <si>
+    <t>MIJ OV</t>
   </si>
 </sst>
 </file>
@@ -430,9 +475,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -749,10 +797,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB9555E0-3443-4710-AD14-3A977E907E6B}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -763,7 +811,7 @@
     <col min="7" max="7" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -789,16 +837,13 @@
         <v>62</v>
       </c>
       <c r="I1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="J1" t="s">
-        <v>68</v>
-      </c>
-      <c r="K1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>100</v>
       </c>
@@ -806,13 +851,13 @@
         <v>10</v>
       </c>
       <c r="C2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" t="s">
         <v>64</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>65</v>
-      </c>
-      <c r="E2" t="s">
-        <v>66</v>
       </c>
       <c r="F2" t="b">
         <v>1</v>
@@ -823,14 +868,222 @@
       <c r="H2">
         <v>0.01</v>
       </c>
-      <c r="I2" t="s">
-        <v>67</v>
-      </c>
-      <c r="J2" t="b">
+      <c r="I2" t="b">
         <v>1</v>
       </c>
-      <c r="K2" t="s">
+      <c r="J2" t="s">
         <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DD3CC7F-96FA-4722-9354-DA6065EED849}">
+  <dimension ref="A1:B24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.140625" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>99</v>
+      </c>
+      <c r="B7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B10">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B11">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>82</v>
+      </c>
+      <c r="B12">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>83</v>
+      </c>
+      <c r="B13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>86</v>
+      </c>
+      <c r="B15" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>101</v>
+      </c>
+      <c r="B16">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>88</v>
+      </c>
+      <c r="B17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>89</v>
+      </c>
+      <c r="B18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>90</v>
+      </c>
+      <c r="B19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>91</v>
+      </c>
+      <c r="B20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>92</v>
+      </c>
+      <c r="B21" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>103</v>
+      </c>
+      <c r="B22" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>93</v>
+      </c>
+      <c r="B23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>94</v>
+      </c>
+      <c r="B24">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -839,11 +1092,106 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21FFED35-A9FD-48DB-B137-EE60E86B3C7B}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7757E3CE-16FD-40F5-A230-112008D36DE8}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.85546875" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" s="2"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27E157EC-B8A8-4DD4-B0B0-EC0F5BEAABD9}">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F4"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -928,7 +1276,377 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6486BE4A-F285-45A5-8B7B-0E738AE5C353}">
+  <dimension ref="A1:C24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B67183C1-66AD-4636-988C-6C4146A80519}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B5" t="s">
+        <v>122</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B22162FB-19FC-4D35-A378-DB18D18AE0D2}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="2" max="2" width="21" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" t="s">
+        <v>112</v>
+      </c>
+      <c r="E4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B8BC91C-7A6C-4F7B-A16D-D5B583B31017}">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C74130A8-7C80-4EF0-924A-78FEEA1CDE59}">
   <dimension ref="A1:F6"/>
   <sheetViews>
@@ -953,16 +1671,16 @@
         <v>51</v>
       </c>
       <c r="C1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D1" t="s">
         <v>50</v>
       </c>
       <c r="E1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" t="s">
         <v>69</v>
-      </c>
-      <c r="F1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -970,7 +1688,7 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C2">
         <v>2022</v>
@@ -979,7 +1697,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
@@ -990,7 +1708,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C3">
         <v>2022</v>
@@ -1015,7 +1733,7 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C5">
         <v>2019</v>
@@ -1033,532 +1751,6 @@
       </c>
       <c r="D6" t="b">
         <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6486BE4A-F285-45A5-8B7B-0E738AE5C353}">
-  <dimension ref="A1:B24"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>26</v>
-      </c>
-      <c r="B19" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>26</v>
-      </c>
-      <c r="B21" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>26</v>
-      </c>
-      <c r="B22" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>26</v>
-      </c>
-      <c r="B23" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24" t="s">
-        <v>44</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21FFED35-A9FD-48DB-B137-EE60E86B3C7B}">
-  <dimension ref="A1:A4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DD3CC7F-96FA-4722-9354-DA6065EED849}">
-  <dimension ref="A1:B24"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="31.140625" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>99</v>
-      </c>
-      <c r="B2">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>98</v>
-      </c>
-      <c r="B3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>100</v>
-      </c>
-      <c r="B6">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>101</v>
-      </c>
-      <c r="B7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>102</v>
-      </c>
-      <c r="B8" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>80</v>
-      </c>
-      <c r="B9" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>82</v>
-      </c>
-      <c r="B10">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>83</v>
-      </c>
-      <c r="B11">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>84</v>
-      </c>
-      <c r="B12">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>85</v>
-      </c>
-      <c r="B13">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>86</v>
-      </c>
-      <c r="B14" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>88</v>
-      </c>
-      <c r="B15" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>103</v>
-      </c>
-      <c r="B16">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>90</v>
-      </c>
-      <c r="B17" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>91</v>
-      </c>
-      <c r="B18" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>92</v>
-      </c>
-      <c r="B19" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>93</v>
-      </c>
-      <c r="B20" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>94</v>
-      </c>
-      <c r="B21" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>105</v>
-      </c>
-      <c r="B22" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>95</v>
-      </c>
-      <c r="B23" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>96</v>
-      </c>
-      <c r="B24">
-        <v>66</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B22162FB-19FC-4D35-A378-DB18D18AE0D2}">
-  <dimension ref="A1:E4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" customWidth="1"/>
-    <col min="5" max="5" width="16" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D1" t="s">
-        <v>109</v>
-      </c>
-      <c r="E1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" t="s">
-        <v>114</v>
-      </c>
-      <c r="E4" t="s">
-        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ondersteuning toegevoegd voor meerdere weegfactoren per variabele. Controle voor instellingen van vorige sessies uitgebreid en verbeterd. Verbergen van cellen met een te laag aantal aangepast.
</commit_message>
<xml_diff>
--- a/configuratie.xlsx
+++ b/configuratie.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ggdnog-my.sharepoint.com/personal/a_dijkstra_ggdnog_nl/Documents/Documenten/Tabellenboek/GGData_tabellenboek/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="136" documentId="8_{0F18ABD2-A895-4412-9B00-D736EAC011EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FAAC9A4E-7792-45BF-AD6C-4E5507B8555D}"/>
+  <xr:revisionPtr revIDLastSave="142" documentId="8_{0F18ABD2-A895-4412-9B00-D736EAC011EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4B9F5287-919F-4B60-9DC4-628443AFC10E}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
   </bookViews>
   <sheets>
     <sheet name="algemeen" sheetId="5" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="132">
   <si>
     <t>naam_dataset</t>
   </si>
@@ -435,6 +435,12 @@
   </si>
   <si>
     <t>MIJ OV</t>
+  </si>
+  <si>
+    <t>weegfactor.d1</t>
+  </si>
+  <si>
+    <t>weegfactor.d2</t>
   </si>
 </sst>
 </file>
@@ -803,15 +809,15 @@
       <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.453125" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" customWidth="1"/>
+    <col min="6" max="6" width="15.453125" customWidth="1"/>
+    <col min="7" max="7" width="11.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -843,7 +849,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>100</v>
       </c>
@@ -888,13 +894,13 @@
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="31.140625" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.1796875" customWidth="1"/>
+    <col min="2" max="2" width="9.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -902,7 +908,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>97</v>
       </c>
@@ -910,7 +916,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>96</v>
       </c>
@@ -918,7 +924,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>95</v>
       </c>
@@ -926,7 +932,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>76</v>
       </c>
@@ -934,7 +940,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>98</v>
       </c>
@@ -942,7 +948,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>99</v>
       </c>
@@ -950,7 +956,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>100</v>
       </c>
@@ -958,7 +964,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>78</v>
       </c>
@@ -966,7 +972,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>80</v>
       </c>
@@ -974,7 +980,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>81</v>
       </c>
@@ -982,7 +988,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>82</v>
       </c>
@@ -990,7 +996,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>83</v>
       </c>
@@ -998,7 +1004,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>84</v>
       </c>
@@ -1006,7 +1012,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>86</v>
       </c>
@@ -1014,7 +1020,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>101</v>
       </c>
@@ -1022,7 +1028,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>88</v>
       </c>
@@ -1030,7 +1036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>89</v>
       </c>
@@ -1038,7 +1044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>90</v>
       </c>
@@ -1046,7 +1052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>91</v>
       </c>
@@ -1054,7 +1060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>92</v>
       </c>
@@ -1062,7 +1068,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>103</v>
       </c>
@@ -1070,7 +1076,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>93</v>
       </c>
@@ -1078,7 +1084,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>94</v>
       </c>
@@ -1099,24 +1105,24 @@
       <selection sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>48</v>
       </c>
@@ -1134,13 +1140,13 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="1" max="1" width="25.81640625" customWidth="1"/>
+    <col min="2" max="2" width="22.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>120</v>
       </c>
@@ -1148,7 +1154,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>124</v>
       </c>
@@ -1156,7 +1162,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>126</v>
       </c>
@@ -1164,7 +1170,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>128</v>
       </c>
@@ -1172,13 +1178,13 @@
         <v>129</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B7" s="2"/>
     </row>
   </sheetData>
@@ -1194,16 +1200,16 @@
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" customWidth="1"/>
-    <col min="2" max="2" width="38.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1"/>
-    <col min="4" max="4" width="27.42578125" customWidth="1"/>
-    <col min="5" max="5" width="23.28515625" customWidth="1"/>
+    <col min="1" max="1" width="17.54296875" customWidth="1"/>
+    <col min="2" max="2" width="38.7265625" customWidth="1"/>
+    <col min="3" max="3" width="15.1796875" customWidth="1"/>
+    <col min="4" max="4" width="27.453125" customWidth="1"/>
+    <col min="5" max="5" width="23.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1220,7 +1226,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1237,7 +1243,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1254,7 +1260,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1278,19 +1284,19 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6486BE4A-F285-45A5-8B7B-0E738AE5C353}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -1298,10 +1304,13 @@
         <v>18</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+      <c r="D1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1309,7 +1318,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1317,12 +1326,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1330,7 +1339,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -1338,7 +1347,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -1346,7 +1355,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -1354,7 +1363,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -1362,7 +1371,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -1370,7 +1379,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -1378,7 +1387,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -1386,7 +1395,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -1394,7 +1403,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -1402,7 +1411,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -1410,7 +1419,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -1418,7 +1427,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -1426,7 +1435,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -1434,7 +1443,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -1442,7 +1451,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -1450,7 +1459,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -1458,7 +1467,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -1466,7 +1475,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -1474,7 +1483,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -1495,9 +1504,9 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -1505,7 +1514,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1513,12 +1522,12 @@
         <v>119</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>120</v>
       </c>
@@ -1526,7 +1535,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>120</v>
       </c>
@@ -1547,16 +1556,16 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="22.7265625" customWidth="1"/>
+    <col min="4" max="4" width="18.7265625" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -1573,7 +1582,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -1587,7 +1596,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>27</v>
       </c>
@@ -1595,7 +1604,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -1619,12 +1628,12 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" customWidth="1"/>
+    <col min="1" max="1" width="24.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>114</v>
       </c>
@@ -1654,16 +1663,16 @@
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="14.7265625" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="17.26953125" customWidth="1"/>
+    <col min="4" max="4" width="14.26953125" customWidth="1"/>
+    <col min="5" max="5" width="13.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>49</v>
       </c>
@@ -1683,7 +1692,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1703,7 +1712,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1717,7 +1726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1728,7 +1737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1742,7 +1751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Variabelelabels toegevoegd aan configuratie.
</commit_message>
<xml_diff>
--- a/configuratie.xlsx
+++ b/configuratie.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ggdnog-my.sharepoint.com/personal/a_dijkstra_ggdnog_nl/Documents/Documenten/Tabellenboek/GGData_tabellenboek/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="142" documentId="8_{0F18ABD2-A895-4412-9B00-D736EAC011EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4B9F5287-919F-4B60-9DC4-628443AFC10E}"/>
+  <xr:revisionPtr revIDLastSave="144" documentId="8_{0F18ABD2-A895-4412-9B00-D736EAC011EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9DAA35F9-7D93-4009-90CA-9746FB020E6F}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
   </bookViews>
   <sheets>
     <sheet name="algemeen" sheetId="5" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="133">
   <si>
     <t>naam_dataset</t>
   </si>
@@ -441,6 +441,9 @@
   </si>
   <si>
     <t>weegfactor.d2</t>
+  </si>
+  <si>
+    <t>vergelijk_variabelelabels</t>
   </si>
 </sst>
 </file>
@@ -803,21 +806,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB9555E0-3443-4710-AD14-3A977E907E6B}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.453125" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="6" max="6" width="15.453125" customWidth="1"/>
-    <col min="7" max="7" width="11.54296875" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -848,8 +852,11 @@
       <c r="J1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>100</v>
       </c>
@@ -879,6 +886,9 @@
       </c>
       <c r="J2" t="s">
         <v>8</v>
+      </c>
+      <c r="K2" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -894,13 +904,13 @@
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.1796875" customWidth="1"/>
-    <col min="2" max="2" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.140625" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -908,7 +918,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>97</v>
       </c>
@@ -916,7 +926,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>96</v>
       </c>
@@ -924,7 +934,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>95</v>
       </c>
@@ -932,7 +942,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>76</v>
       </c>
@@ -940,7 +950,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>98</v>
       </c>
@@ -948,7 +958,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>99</v>
       </c>
@@ -956,7 +966,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>100</v>
       </c>
@@ -964,7 +974,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>78</v>
       </c>
@@ -972,7 +982,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>80</v>
       </c>
@@ -980,7 +990,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>81</v>
       </c>
@@ -988,7 +998,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>82</v>
       </c>
@@ -996,7 +1006,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>83</v>
       </c>
@@ -1004,7 +1014,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>84</v>
       </c>
@@ -1012,7 +1022,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>86</v>
       </c>
@@ -1020,7 +1030,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>101</v>
       </c>
@@ -1028,7 +1038,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>88</v>
       </c>
@@ -1036,7 +1046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>89</v>
       </c>
@@ -1044,7 +1054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>90</v>
       </c>
@@ -1052,7 +1062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>91</v>
       </c>
@@ -1060,7 +1070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>92</v>
       </c>
@@ -1068,7 +1078,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>103</v>
       </c>
@@ -1076,7 +1086,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>93</v>
       </c>
@@ -1084,7 +1094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>94</v>
       </c>
@@ -1105,24 +1115,24 @@
       <selection sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>48</v>
       </c>
@@ -1140,13 +1150,13 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.81640625" customWidth="1"/>
-    <col min="2" max="2" width="22.1796875" customWidth="1"/>
+    <col min="1" max="1" width="25.85546875" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>120</v>
       </c>
@@ -1154,7 +1164,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>124</v>
       </c>
@@ -1162,7 +1172,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>126</v>
       </c>
@@ -1170,7 +1180,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>128</v>
       </c>
@@ -1178,13 +1188,13 @@
         <v>129</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
     </row>
   </sheetData>
@@ -1200,16 +1210,16 @@
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.54296875" customWidth="1"/>
-    <col min="2" max="2" width="38.7265625" customWidth="1"/>
-    <col min="3" max="3" width="15.1796875" customWidth="1"/>
-    <col min="4" max="4" width="27.453125" customWidth="1"/>
-    <col min="5" max="5" width="23.26953125" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+    <col min="2" max="2" width="38.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1226,7 +1236,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1243,7 +1253,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1260,7 +1270,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1286,17 +1296,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6486BE4A-F285-45A5-8B7B-0E738AE5C353}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="12.54296875" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -1310,7 +1320,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1318,7 +1328,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1326,12 +1336,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1339,7 +1349,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -1347,7 +1357,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -1355,7 +1365,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -1363,7 +1373,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -1371,7 +1381,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -1379,7 +1389,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -1387,7 +1397,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -1395,7 +1405,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -1403,7 +1413,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -1411,7 +1421,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -1419,7 +1429,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -1427,7 +1437,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -1435,7 +1445,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -1443,7 +1453,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -1451,7 +1461,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -1459,7 +1469,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -1467,7 +1477,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -1475,7 +1485,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -1483,7 +1493,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -1504,9 +1514,9 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -1514,7 +1524,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1522,12 +1532,12 @@
         <v>119</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>120</v>
       </c>
@@ -1535,7 +1545,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>120</v>
       </c>
@@ -1556,16 +1566,16 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="22.7265625" customWidth="1"/>
-    <col min="4" max="4" width="18.7265625" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -1582,7 +1592,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -1596,7 +1606,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>27</v>
       </c>
@@ -1604,7 +1614,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -1628,12 +1638,12 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.26953125" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>114</v>
       </c>
@@ -1663,16 +1673,16 @@
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.7265625" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="17.26953125" customWidth="1"/>
-    <col min="4" max="4" width="14.26953125" customWidth="1"/>
-    <col min="5" max="5" width="13.81640625" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>49</v>
       </c>
@@ -1692,7 +1702,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1712,7 +1722,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1726,7 +1736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1737,7 +1747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1751,7 +1761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Dichotoom/niet dichotoom toegevoegd. Log levels toegevoegd. Forceren van datatypen toegevoegd. Probleem opgelost waarbij data van de VO monitor zorgt voor problemen door de omzetting naar strings van gemeentecodes.
</commit_message>
<xml_diff>
--- a/configuratie.xlsx
+++ b/configuratie.xlsx
@@ -8,21 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ggdnog-my.sharepoint.com/personal/a_dijkstra_ggdnog_nl/Documents/Documenten/Tabellenboek/GGData_tabellenboek/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="144" documentId="8_{0F18ABD2-A895-4412-9B00-D736EAC011EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9DAA35F9-7D93-4009-90CA-9746FB020E6F}"/>
+  <xr:revisionPtr revIDLastSave="146" documentId="8_{0F18ABD2-A895-4412-9B00-D736EAC011EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C760BA6C-561C-4DB4-9BFE-D40D289AB2A3}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
   </bookViews>
   <sheets>
     <sheet name="algemeen" sheetId="5" r:id="rId1"/>
     <sheet name="crossings" sheetId="3" r:id="rId2"/>
-    <sheet name="headers_afkortingen" sheetId="10" r:id="rId3"/>
-    <sheet name="datasets" sheetId="1" r:id="rId4"/>
-    <sheet name="indeling_rijen" sheetId="2" r:id="rId5"/>
-    <sheet name="intro_tekst" sheetId="9" r:id="rId6"/>
-    <sheet name="labelcorrectie" sheetId="7" r:id="rId7"/>
-    <sheet name="logos" sheetId="8" r:id="rId8"/>
-    <sheet name="onderdelen" sheetId="4" r:id="rId9"/>
-    <sheet name="opmaak" sheetId="6" r:id="rId10"/>
+    <sheet name="datasets" sheetId="1" r:id="rId3"/>
+    <sheet name="dichotoom" sheetId="11" r:id="rId4"/>
+    <sheet name="niet_dichotoom" sheetId="12" r:id="rId5"/>
+    <sheet name="headers_afkortingen" sheetId="10" r:id="rId6"/>
+    <sheet name="indeling_rijen" sheetId="2" r:id="rId7"/>
+    <sheet name="intro_tekst" sheetId="9" r:id="rId8"/>
+    <sheet name="labelcorrectie" sheetId="7" r:id="rId9"/>
+    <sheet name="logos" sheetId="8" r:id="rId10"/>
+    <sheet name="onderdelen" sheetId="4" r:id="rId11"/>
+    <sheet name="opmaak" sheetId="6" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="134">
   <si>
     <t>naam_dataset</t>
   </si>
@@ -444,6 +446,9 @@
   </si>
   <si>
     <t>vergelijk_variabelelabels</t>
+  </si>
+  <si>
+    <t>variabele</t>
   </si>
 </sst>
 </file>
@@ -808,8 +813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB9555E0-3443-4710-AD14-3A977E907E6B}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -897,6 +902,153 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B8BC91C-7A6C-4F7B-A16D-D5B583B31017}">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C74130A8-7C80-4EF0-924A-78FEEA1CDE59}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="21" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2">
+        <v>2022</v>
+      </c>
+      <c r="D2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3">
+        <v>2022</v>
+      </c>
+      <c r="D3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>2022</v>
+      </c>
+      <c r="D4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5">
+        <v>2019</v>
+      </c>
+      <c r="D5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>2022</v>
+      </c>
+      <c r="D6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DD3CC7F-96FA-4722-9354-DA6065EED849}">
   <dimension ref="A1:B24"/>
   <sheetViews>
@@ -1143,6 +1295,136 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27E157EC-B8A8-4DD4-B0B0-EC0F5BEAABD9}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+    <col min="2" max="2" width="38.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6B9AAB2-B21C-4F9A-AA85-AAC79B043700}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38BC63A0-66D1-48A8-8EE0-6CAC0789D923}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7757E3CE-16FD-40F5-A230-112008D36DE8}">
   <dimension ref="A1:B7"/>
   <sheetViews>
@@ -1202,97 +1484,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27E157EC-B8A8-4DD4-B0B0-EC0F5BEAABD9}">
-  <dimension ref="A1:E4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.5703125" customWidth="1"/>
-    <col min="2" max="2" width="38.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1"/>
-    <col min="4" max="4" width="27.42578125" customWidth="1"/>
-    <col min="5" max="5" width="23.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6486BE4A-F285-45A5-8B7B-0E738AE5C353}">
   <dimension ref="A1:D24"/>
   <sheetViews>
@@ -1506,7 +1698,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B67183C1-66AD-4636-988C-6C4146A80519}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -1558,7 +1750,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B22162FB-19FC-4D35-A378-DB18D18AE0D2}">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -1628,151 +1820,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B8BC91C-7A6C-4F7B-A16D-D5B583B31017}">
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="24.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>114</v>
-      </c>
-      <c r="B1" t="s">
-        <v>115</v>
-      </c>
-      <c r="C1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D1" t="s">
-        <v>117</v>
-      </c>
-      <c r="E1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C74130A8-7C80-4EF0-924A-78FEEA1CDE59}">
-  <dimension ref="A1:F6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C2">
-        <v>2022</v>
-      </c>
-      <c r="D2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C3">
-        <v>2022</v>
-      </c>
-      <c r="D3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4">
-        <v>2022</v>
-      </c>
-      <c r="D4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C5">
-        <v>2019</v>
-      </c>
-      <c r="D5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6">
-        <v>2022</v>
-      </c>
-      <c r="D6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Forceer_datatypen ingebouwd en gecorrigeerd.
</commit_message>
<xml_diff>
--- a/configuratie.xlsx
+++ b/configuratie.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ggdnog-my.sharepoint.com/personal/a_dijkstra_ggdnog_nl/Documents/Documenten/Tabellenboek/GGData_tabellenboek/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="146" documentId="8_{0F18ABD2-A895-4412-9B00-D736EAC011EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C760BA6C-561C-4DB4-9BFE-D40D289AB2A3}"/>
+  <xr:revisionPtr revIDLastSave="148" documentId="8_{0F18ABD2-A895-4412-9B00-D736EAC011EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D8B4DF7-783E-492D-92B5-ED9C3A9798A9}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
   </bookViews>
   <sheets>
     <sheet name="algemeen" sheetId="5" r:id="rId1"/>
@@ -18,13 +18,14 @@
     <sheet name="datasets" sheetId="1" r:id="rId3"/>
     <sheet name="dichotoom" sheetId="11" r:id="rId4"/>
     <sheet name="niet_dichotoom" sheetId="12" r:id="rId5"/>
-    <sheet name="headers_afkortingen" sheetId="10" r:id="rId6"/>
-    <sheet name="indeling_rijen" sheetId="2" r:id="rId7"/>
-    <sheet name="intro_tekst" sheetId="9" r:id="rId8"/>
-    <sheet name="labelcorrectie" sheetId="7" r:id="rId9"/>
-    <sheet name="logos" sheetId="8" r:id="rId10"/>
-    <sheet name="onderdelen" sheetId="4" r:id="rId11"/>
-    <sheet name="opmaak" sheetId="6" r:id="rId12"/>
+    <sheet name="forceer_datatypen" sheetId="13" r:id="rId6"/>
+    <sheet name="headers_afkortingen" sheetId="10" r:id="rId7"/>
+    <sheet name="indeling_rijen" sheetId="2" r:id="rId8"/>
+    <sheet name="intro_tekst" sheetId="9" r:id="rId9"/>
+    <sheet name="labelcorrectie" sheetId="7" r:id="rId10"/>
+    <sheet name="logos" sheetId="8" r:id="rId11"/>
+    <sheet name="onderdelen" sheetId="4" r:id="rId12"/>
+    <sheet name="opmaak" sheetId="6" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="134">
   <si>
     <t>naam_dataset</t>
   </si>
@@ -902,6 +903,78 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B22162FB-19FC-4D35-A378-DB18D18AE0D2}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="2" max="2" width="21" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" t="s">
+        <v>112</v>
+      </c>
+      <c r="E4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B8BC91C-7A6C-4F7B-A16D-D5B583B31017}">
   <dimension ref="A1:E1"/>
   <sheetViews>
@@ -936,7 +1009,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C74130A8-7C80-4EF0-924A-78FEEA1CDE59}">
   <dimension ref="A1:F6"/>
   <sheetViews>
@@ -1048,7 +1121,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DD3CC7F-96FA-4722-9354-DA6065EED849}">
   <dimension ref="A1:B24"/>
   <sheetViews>
@@ -1408,7 +1481,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38BC63A0-66D1-48A8-8EE0-6CAC0789D923}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1425,6 +1498,29 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9C5E0E0-AEC7-4A98-8EDA-BFF72DE4F63D}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7757E3CE-16FD-40F5-A230-112008D36DE8}">
   <dimension ref="A1:B7"/>
   <sheetViews>
@@ -1484,7 +1580,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6486BE4A-F285-45A5-8B7B-0E738AE5C353}">
   <dimension ref="A1:D24"/>
   <sheetViews>
@@ -1698,7 +1794,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B67183C1-66AD-4636-988C-6C4146A80519}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -1748,76 +1844,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B22162FB-19FC-4D35-A378-DB18D18AE0D2}">
-  <dimension ref="A1:E4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" customWidth="1"/>
-    <col min="5" max="5" width="16" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D1" t="s">
-        <v>107</v>
-      </c>
-      <c r="E1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" t="s">
-        <v>112</v>
-      </c>
-      <c r="E4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Fout bij het weergeven van aantallen gecorrigeerd. Optimalisatie van herkenning dubbele resultaten.
</commit_message>
<xml_diff>
--- a/configuratie.xlsx
+++ b/configuratie.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ggdnog-my.sharepoint.com/personal/a_dijkstra_ggdnog_nl/Documents/Documenten/Tabellenboek/GGData_tabellenboek/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="148" documentId="8_{0F18ABD2-A895-4412-9B00-D736EAC011EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D8B4DF7-783E-492D-92B5-ED9C3A9798A9}"/>
+  <xr:revisionPtr revIDLastSave="150" documentId="8_{0F18ABD2-A895-4412-9B00-D736EAC011EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B52A998A-4AE6-4D7C-83D9-C55B49F63702}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
   </bookViews>
   <sheets>
     <sheet name="algemeen" sheetId="5" r:id="rId1"/>
@@ -814,20 +814,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB9555E0-3443-4710-AD14-3A977E907E6B}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.453125" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" customWidth="1"/>
-    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.453125" customWidth="1"/>
+    <col min="7" max="7" width="11.54296875" customWidth="1"/>
+    <col min="11" max="11" width="9.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -862,12 +862,12 @@
         <v>132</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
         <v>63</v>
@@ -910,16 +910,16 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="22.7265625" customWidth="1"/>
+    <col min="4" max="4" width="18.7265625" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -936,7 +936,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -950,7 +950,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>27</v>
       </c>
@@ -958,7 +958,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -982,12 +982,12 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" customWidth="1"/>
+    <col min="1" max="1" width="24.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>114</v>
       </c>
@@ -1017,16 +1017,16 @@
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="14.7265625" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="17.26953125" customWidth="1"/>
+    <col min="4" max="4" width="14.26953125" customWidth="1"/>
+    <col min="5" max="5" width="13.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>49</v>
       </c>
@@ -1046,7 +1046,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1066,7 +1066,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1080,7 +1080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1091,7 +1091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1105,7 +1105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1129,13 +1129,13 @@
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="31.140625" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.1796875" customWidth="1"/>
+    <col min="2" max="2" width="9.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -1143,7 +1143,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>97</v>
       </c>
@@ -1151,7 +1151,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>96</v>
       </c>
@@ -1159,7 +1159,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>95</v>
       </c>
@@ -1167,7 +1167,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>76</v>
       </c>
@@ -1175,7 +1175,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>98</v>
       </c>
@@ -1183,7 +1183,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>99</v>
       </c>
@@ -1191,7 +1191,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>100</v>
       </c>
@@ -1199,7 +1199,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>78</v>
       </c>
@@ -1207,7 +1207,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>80</v>
       </c>
@@ -1215,7 +1215,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>81</v>
       </c>
@@ -1223,7 +1223,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>82</v>
       </c>
@@ -1231,7 +1231,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>83</v>
       </c>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>84</v>
       </c>
@@ -1247,7 +1247,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>86</v>
       </c>
@@ -1255,7 +1255,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>101</v>
       </c>
@@ -1263,7 +1263,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>88</v>
       </c>
@@ -1271,7 +1271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>89</v>
       </c>
@@ -1279,7 +1279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>90</v>
       </c>
@@ -1287,7 +1287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>91</v>
       </c>
@@ -1295,7 +1295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>92</v>
       </c>
@@ -1303,7 +1303,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>103</v>
       </c>
@@ -1311,7 +1311,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>93</v>
       </c>
@@ -1319,7 +1319,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>94</v>
       </c>
@@ -1340,24 +1340,24 @@
       <selection sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>48</v>
       </c>
@@ -1375,16 +1375,16 @@
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" customWidth="1"/>
-    <col min="2" max="2" width="38.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1"/>
-    <col min="4" max="4" width="27.42578125" customWidth="1"/>
-    <col min="5" max="5" width="23.28515625" customWidth="1"/>
+    <col min="1" max="1" width="17.54296875" customWidth="1"/>
+    <col min="2" max="2" width="38.7265625" customWidth="1"/>
+    <col min="3" max="3" width="15.1796875" customWidth="1"/>
+    <col min="4" max="4" width="27.453125" customWidth="1"/>
+    <col min="5" max="5" width="23.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1401,7 +1401,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1418,7 +1418,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1435,7 +1435,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1465,9 +1465,9 @@
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>133</v>
       </c>
@@ -1485,9 +1485,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>133</v>
       </c>
@@ -1501,13 +1501,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9C5E0E0-AEC7-4A98-8EDA-BFF72DE4F63D}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>133</v>
       </c>
@@ -1528,13 +1528,13 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="1" max="1" width="25.81640625" customWidth="1"/>
+    <col min="2" max="2" width="22.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>120</v>
       </c>
@@ -1542,7 +1542,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>124</v>
       </c>
@@ -1550,7 +1550,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>126</v>
       </c>
@@ -1558,7 +1558,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>128</v>
       </c>
@@ -1566,13 +1566,13 @@
         <v>129</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B7" s="2"/>
     </row>
   </sheetData>
@@ -1588,13 +1588,13 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -1608,7 +1608,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1616,7 +1616,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1624,12 +1624,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1637,7 +1637,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -1645,7 +1645,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -1653,7 +1653,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -1661,7 +1661,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -1669,7 +1669,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -1677,7 +1677,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -1685,7 +1685,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -1693,7 +1693,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -1701,7 +1701,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -1709,7 +1709,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -1717,7 +1717,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -1725,7 +1725,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -1733,7 +1733,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -1741,7 +1741,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -1749,7 +1749,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -1757,7 +1757,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -1765,7 +1765,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -1773,7 +1773,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -1781,7 +1781,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -1802,9 +1802,9 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -1812,7 +1812,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1820,12 +1820,12 @@
         <v>119</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>120</v>
       </c>
@@ -1833,7 +1833,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>120</v>
       </c>

</xml_diff>

<commit_message>
Logging toegevoegd aan het script, zodat meldingen beter leesbaar zijn.
</commit_message>
<xml_diff>
--- a/configuratie.xlsx
+++ b/configuratie.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ggdnog-my.sharepoint.com/personal/a_dijkstra_ggdnog_nl/Documents/Documenten/Tabellenboek/GGData_tabellenboek/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="150" documentId="8_{0F18ABD2-A895-4412-9B00-D736EAC011EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B52A998A-4AE6-4D7C-83D9-C55B49F63702}"/>
+  <xr:revisionPtr revIDLastSave="157" documentId="8_{0F18ABD2-A895-4412-9B00-D736EAC011EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4463FE5-FF2B-4B16-8024-B414E1DF4784}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="5" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
   </bookViews>
   <sheets>
     <sheet name="algemeen" sheetId="5" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="135">
   <si>
     <t>naam_dataset</t>
   </si>
@@ -450,6 +450,9 @@
   </si>
   <si>
     <t>variabele</t>
+  </si>
+  <si>
+    <t>numeric</t>
   </si>
 </sst>
 </file>
@@ -814,7 +817,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB9555E0-3443-4710-AD14-3A977E907E6B}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -1126,7 +1129,7 @@
   <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1499,13 +1502,16 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9C5E0E0-AEC7-4A98-8EDA-BFF72DE4F63D}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.90625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -1513,6 +1519,14 @@
       </c>
       <c r="B1" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aparte opmaak voor vraag en kop toegevoegd.
</commit_message>
<xml_diff>
--- a/configuratie.xlsx
+++ b/configuratie.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ggdnog-my.sharepoint.com/personal/a_dijkstra_ggdnog_nl/Documents/Documenten/Tabellenboek/GGData_tabellenboek/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="157" documentId="8_{0F18ABD2-A895-4412-9B00-D736EAC011EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4463FE5-FF2B-4B16-8024-B414E1DF4784}"/>
+  <xr:revisionPtr revIDLastSave="182" documentId="8_{0F18ABD2-A895-4412-9B00-D736EAC011EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{25FA46AB-06E1-4ED4-AA0C-241F12A0BC5D}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="5" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="7" activeTab="7" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
   </bookViews>
   <sheets>
     <sheet name="algemeen" sheetId="5" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="144">
   <si>
     <t>naam_dataset</t>
   </si>
@@ -453,6 +453,33 @@
   </si>
   <si>
     <t>numeric</t>
+  </si>
+  <si>
+    <t>weergave</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>kolomkoppen</t>
+  </si>
+  <si>
+    <t>vraag_size</t>
+  </si>
+  <si>
+    <t>vraag_color</t>
+  </si>
+  <si>
+    <t>vraag_decoration</t>
+  </si>
+  <si>
+    <t>vraag_fill</t>
+  </si>
+  <si>
+    <t>vraag</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -815,10 +842,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB9555E0-3443-4710-AD14-3A977E907E6B}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -830,7 +857,7 @@
     <col min="11" max="11" width="9.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -864,8 +891,11 @@
       <c r="K1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>10</v>
       </c>
@@ -898,6 +928,9 @@
       </c>
       <c r="K2" t="b">
         <v>0</v>
+      </c>
+      <c r="L2" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -1126,10 +1159,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DD3CC7F-96FA-4722-9354-DA6065EED849}">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1212,121 +1245,153 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>80</v>
+        <v>138</v>
       </c>
       <c r="B10">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>81</v>
-      </c>
-      <c r="B11">
-        <v>28</v>
+        <v>139</v>
+      </c>
+      <c r="B11" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>82</v>
-      </c>
-      <c r="B12">
-        <v>60</v>
+        <v>140</v>
+      </c>
+      <c r="B12" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>83</v>
-      </c>
-      <c r="B13">
-        <v>10</v>
+        <v>141</v>
+      </c>
+      <c r="B13" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>84</v>
-      </c>
-      <c r="B14" t="s">
-        <v>85</v>
+        <v>80</v>
+      </c>
+      <c r="B14">
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>86</v>
-      </c>
-      <c r="B15" t="s">
-        <v>87</v>
+        <v>81</v>
+      </c>
+      <c r="B15">
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="B16">
-        <v>11</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>88</v>
-      </c>
-      <c r="B17" t="b">
-        <v>0</v>
+        <v>83</v>
+      </c>
+      <c r="B17">
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>89</v>
-      </c>
-      <c r="B18" t="b">
-        <v>0</v>
+        <v>84</v>
+      </c>
+      <c r="B18" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>90</v>
-      </c>
-      <c r="B19" t="b">
-        <v>0</v>
+        <v>86</v>
+      </c>
+      <c r="B19" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>91</v>
-      </c>
-      <c r="B20" t="b">
-        <v>1</v>
+        <v>101</v>
+      </c>
+      <c r="B20">
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>92</v>
-      </c>
-      <c r="B21" t="s">
-        <v>102</v>
+        <v>88</v>
+      </c>
+      <c r="B21" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>103</v>
-      </c>
-      <c r="B22" t="s">
-        <v>104</v>
+        <v>89</v>
+      </c>
+      <c r="B22" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
+        <v>91</v>
+      </c>
+      <c r="B24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>92</v>
+      </c>
+      <c r="B25" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>103</v>
+      </c>
+      <c r="B26" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>93</v>
+      </c>
+      <c r="B27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
         <v>94</v>
       </c>
-      <c r="B24">
+      <c r="B28">
         <v>66</v>
       </c>
     </row>
@@ -1504,13 +1569,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9C5E0E0-AEC7-4A98-8EDA-BFF72DE4F63D}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.90625" customWidth="1"/>
+    <col min="1" max="1" width="15.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -1596,19 +1661,19 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6486BE4A-F285-45A5-8B7B-0E738AE5C353}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="12.54296875" customWidth="1"/>
+    <col min="2" max="3" width="12.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -1616,13 +1681,16 @@
         <v>18</v>
       </c>
       <c r="C1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D1" t="s">
         <v>130</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1630,7 +1698,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1638,12 +1706,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1651,7 +1719,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -1659,7 +1727,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -1667,7 +1735,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -1675,15 +1743,15 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>142</v>
       </c>
       <c r="B9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -1691,7 +1759,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -1699,7 +1767,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -1707,15 +1775,18 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>142</v>
       </c>
       <c r="B13" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C13" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -1723,7 +1794,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -1731,7 +1802,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -1739,7 +1810,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -1747,7 +1818,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -1755,7 +1826,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -1763,7 +1834,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -1771,15 +1842,18 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>26</v>
       </c>
       <c r="B21" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C21" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -1787,7 +1861,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -1795,7 +1869,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
Digitoegankelijkheid uitgebreid en opmaak toegevoegd om overeen te komen met Excelversie.
</commit_message>
<xml_diff>
--- a/configuratie.xlsx
+++ b/configuratie.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ggdnog-my.sharepoint.com/personal/a_dijkstra_ggdnog_nl/Documents/Documenten/Tabellenboek/GGData_tabellenboek/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="182" documentId="8_{0F18ABD2-A895-4412-9B00-D736EAC011EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{25FA46AB-06E1-4ED4-AA0C-241F12A0BC5D}"/>
+  <xr:revisionPtr revIDLastSave="200" documentId="8_{0F18ABD2-A895-4412-9B00-D736EAC011EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1D133B85-06B1-4AAA-B914-13734E399113}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="7" activeTab="7" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
   </bookViews>
   <sheets>
     <sheet name="algemeen" sheetId="5" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="147">
   <si>
     <t>naam_dataset</t>
   </si>
@@ -248,9 +248,6 @@
     <t>-</t>
   </si>
   <si>
-    <t>multithreading</t>
-  </si>
-  <si>
     <t>sign_crossing</t>
   </si>
   <si>
@@ -356,9 +353,6 @@
     <t>font_size</t>
   </si>
   <si>
-    <t>dubbel</t>
-  </si>
-  <si>
     <t>header_template</t>
   </si>
   <si>
@@ -377,12 +371,6 @@
     <t>antwoord_nieuw</t>
   </si>
   <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>Abc</t>
-  </si>
-  <si>
     <t>Alleen opleiding</t>
   </si>
   <si>
@@ -480,6 +468,27 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>Testvervanging</t>
+  </si>
+  <si>
+    <t>Vervangen van 2 waarden</t>
+  </si>
+  <si>
+    <t>enkel</t>
+  </si>
+  <si>
+    <t>afkapwaarde_antwoord</t>
+  </si>
+  <si>
+    <t>template_html</t>
+  </si>
+  <si>
+    <t>template_digitoegankelijk.html</t>
+  </si>
+  <si>
+    <t>vraag_verbergen_bij_missend_antwoord</t>
   </si>
 </sst>
 </file>
@@ -842,22 +851,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB9555E0-3443-4710-AD14-3A977E907E6B}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.453125" customWidth="1"/>
-    <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="6" max="6" width="15.453125" customWidth="1"/>
-    <col min="7" max="7" width="11.54296875" customWidth="1"/>
-    <col min="11" max="11" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="2" max="4" width="16" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" customWidth="1"/>
+    <col min="12" max="12" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -865,72 +878,84 @@
         <v>56</v>
       </c>
       <c r="C1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E1" t="s">
         <v>57</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>58</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>59</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>60</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>61</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>62</v>
       </c>
-      <c r="I1" t="s">
-        <v>66</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>5</v>
       </c>
-      <c r="K1" t="s">
-        <v>132</v>
-      </c>
       <c r="L1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+        <v>128</v>
+      </c>
+      <c r="M1" t="s">
+        <v>144</v>
+      </c>
+      <c r="N1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>10</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
         <v>63</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>64</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>65</v>
       </c>
-      <c r="F2" t="b">
+      <c r="H2" t="b">
         <v>1</v>
       </c>
-      <c r="G2">
+      <c r="I2">
         <v>0</v>
       </c>
-      <c r="H2">
+      <c r="J2">
         <v>0.01</v>
       </c>
-      <c r="I2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>8</v>
       </c>
-      <c r="K2" t="b">
+      <c r="L2" t="b">
         <v>0</v>
       </c>
-      <c r="L2" t="s">
-        <v>136</v>
+      <c r="M2" t="s">
+        <v>145</v>
+      </c>
+      <c r="N2" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -943,66 +968,66 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="22.7265625" customWidth="1"/>
-    <col min="4" max="4" width="18.7265625" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>26</v>
       </c>
       <c r="B1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D1" t="s">
         <v>105</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>106</v>
       </c>
-      <c r="D1" t="s">
-        <v>107</v>
-      </c>
-      <c r="E1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>110</v>
+        <v>141</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E4" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1018,26 +1043,26 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.26953125" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E1" t="s">
         <v>114</v>
-      </c>
-      <c r="B1" t="s">
-        <v>115</v>
-      </c>
-      <c r="C1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D1" t="s">
-        <v>117</v>
-      </c>
-      <c r="E1" t="s">
-        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -1053,16 +1078,16 @@
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.7265625" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="17.26953125" customWidth="1"/>
-    <col min="4" max="4" width="14.26953125" customWidth="1"/>
-    <col min="5" max="5" width="13.81640625" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>49</v>
       </c>
@@ -1070,24 +1095,24 @@
         <v>51</v>
       </c>
       <c r="C1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D1" t="s">
         <v>50</v>
       </c>
       <c r="E1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C2">
         <v>2022</v>
@@ -1096,18 +1121,18 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C3">
         <v>2022</v>
@@ -1116,7 +1141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1127,12 +1152,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C5">
         <v>2019</v>
@@ -1141,7 +1166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1162,234 +1187,234 @@
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.1796875" customWidth="1"/>
-    <col min="2" max="2" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.140625" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
       <c r="B1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B2">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>95</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
         <v>76</v>
       </c>
-      <c r="B5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B6">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>99</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>100</v>
-      </c>
-      <c r="B8" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" t="s">
         <v>78</v>
       </c>
-      <c r="B9" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B10">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>136</v>
+      </c>
+      <c r="B12" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>140</v>
-      </c>
-      <c r="B12" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>79</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>80</v>
       </c>
       <c r="B14">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B15">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B16">
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B17">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>83</v>
+      </c>
+      <c r="B18" t="s">
         <v>84</v>
       </c>
-      <c r="B18" t="s">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+      <c r="B19" t="s">
         <v>86</v>
       </c>
-      <c r="B19" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B20">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B21" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B22" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B23" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B24" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>91</v>
+      </c>
+      <c r="B25" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>101</v>
+      </c>
+      <c r="B26" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>92</v>
-      </c>
-      <c r="B25" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>103</v>
-      </c>
-      <c r="B26" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>93</v>
       </c>
       <c r="B27" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B28">
         <v>66</v>
@@ -1408,24 +1433,24 @@
       <selection sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>48</v>
       </c>
@@ -1443,16 +1468,16 @@
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.54296875" customWidth="1"/>
-    <col min="2" max="2" width="38.7265625" customWidth="1"/>
-    <col min="3" max="3" width="15.1796875" customWidth="1"/>
-    <col min="4" max="4" width="27.453125" customWidth="1"/>
-    <col min="5" max="5" width="23.26953125" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+    <col min="2" max="2" width="38.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1469,7 +1494,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1486,7 +1511,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1503,7 +1528,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1533,11 +1558,11 @@
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -1553,11 +1578,11 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -1573,25 +1598,25 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.81640625" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -1607,51 +1632,51 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.81640625" customWidth="1"/>
-    <col min="2" max="2" width="22.1796875" customWidth="1"/>
+    <col min="1" max="1" width="25.85546875" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>120</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B3" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>124</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B4" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>126</v>
-      </c>
-      <c r="B3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>128</v>
-      </c>
-      <c r="B4" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
     </row>
   </sheetData>
@@ -1663,17 +1688,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6486BE4A-F285-45A5-8B7B-0E738AE5C353}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="3" width="12.54296875" customWidth="1"/>
+    <col min="2" max="3" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -1681,16 +1706,16 @@
         <v>18</v>
       </c>
       <c r="C1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="E1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1698,7 +1723,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1706,12 +1731,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1719,7 +1744,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -1727,7 +1752,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -1735,7 +1760,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -1743,15 +1768,15 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -1759,7 +1784,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -1767,7 +1792,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -1775,18 +1800,18 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B13" t="s">
         <v>33</v>
       </c>
       <c r="C13" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -1794,7 +1819,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -1802,7 +1827,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -1810,7 +1835,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -1818,7 +1843,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -1826,7 +1851,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -1834,7 +1859,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -1842,7 +1867,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -1850,10 +1875,10 @@
         <v>41</v>
       </c>
       <c r="C21" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -1861,7 +1886,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -1869,7 +1894,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -1884,15 +1909,15 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B67183C1-66AD-4636-988C-6C4146A80519}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -1900,33 +1925,38 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B4" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B5" t="s">
-        <v>122</v>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Nieuwe functie toegevoegd: beperkte subset waardes weergeven. Hiervoor nieuwe kolom 'waardes' in tabblad indeling_rijen.
</commit_message>
<xml_diff>
--- a/configuratie.xlsx
+++ b/configuratie.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ggdnog-my.sharepoint.com/personal/a_dijkstra_ggdnog_nl/Documents/Documenten/Tabellenboek/GGData_tabellenboek/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hetservicecentrum-my.sharepoint.com/personal/a_dijkstra_ggdnog_nl/Documents/Documenten/Tabellenboek/GGData_tabellenboek/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="200" documentId="8_{0F18ABD2-A895-4412-9B00-D736EAC011EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1D133B85-06B1-4AAA-B914-13734E399113}"/>
+  <xr:revisionPtr revIDLastSave="203" documentId="8_{0F18ABD2-A895-4412-9B00-D736EAC011EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5DE23485-AE06-41E9-9774-6822B2E38011}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="7" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
   </bookViews>
   <sheets>
     <sheet name="algemeen" sheetId="5" r:id="rId1"/>
@@ -28,6 +28,7 @@
     <sheet name="opmaak" sheetId="6" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="149">
   <si>
     <t>naam_dataset</t>
   </si>
@@ -489,6 +490,12 @@
   </si>
   <si>
     <t>vraag_verbergen_bij_missend_antwoord</t>
+  </si>
+  <si>
+    <t>waardes</t>
+  </si>
+  <si>
+    <t>5,4,3,2,1</t>
   </si>
 </sst>
 </file>
@@ -555,9 +562,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Thema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -595,7 +602,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -701,7 +708,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -843,7 +850,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -853,7 +860,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB9555E0-3443-4710-AD14-3A977E907E6B}">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -1465,7 +1472,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1686,19 +1693,19 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6486BE4A-F285-45A5-8B7B-0E738AE5C353}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="3" width="12.5703125" customWidth="1"/>
+    <col min="2" max="4" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -1706,16 +1713,19 @@
         <v>18</v>
       </c>
       <c r="C1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D1" t="s">
         <v>133</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>126</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1723,7 +1733,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1731,12 +1741,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1744,7 +1754,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -1752,7 +1762,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -1760,15 +1770,18 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
       <c r="B8" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>138</v>
       </c>
@@ -1776,7 +1789,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -1784,7 +1797,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -1792,7 +1805,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -1800,18 +1813,18 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>138</v>
       </c>
       <c r="B13" t="s">
         <v>33</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -1819,7 +1832,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -1827,7 +1840,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -1835,7 +1848,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -1843,7 +1856,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -1851,7 +1864,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -1859,7 +1872,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -1867,18 +1880,18 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>26</v>
       </c>
       <c r="B21" t="s">
         <v>41</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -1886,7 +1899,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -1894,7 +1907,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
Toegevoegd: bold/italic/underline in digitoegankelijke versie, handleiding uitgebreid met veranderingen sinds V&O. Fix: eerste optie in springmenu digitoegankelijke versie werkt weer, aantallen zijn nu gebaseerd op aantal rijen ipv aantal antwoorden.
</commit_message>
<xml_diff>
--- a/configuratie.xlsx
+++ b/configuratie.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hetservicecentrum-my.sharepoint.com/personal/a_dijkstra_ggdnog_nl/Documents/Documenten/Tabellenboek/GGData_tabellenboek/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="203" documentId="8_{0F18ABD2-A895-4412-9B00-D736EAC011EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5DE23485-AE06-41E9-9774-6822B2E38011}"/>
+  <xr:revisionPtr revIDLastSave="206" documentId="8_{0F18ABD2-A895-4412-9B00-D736EAC011EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{37B0C08A-1EA6-4E89-AE27-665A81CDEC4E}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="7" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="7" activeTab="7" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
   </bookViews>
   <sheets>
     <sheet name="algemeen" sheetId="5" r:id="rId1"/>
@@ -28,7 +28,6 @@
     <sheet name="opmaak" sheetId="6" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -49,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="151">
   <si>
     <t>naam_dataset</t>
   </si>
@@ -495,7 +494,13 @@
     <t>waardes</t>
   </si>
   <si>
-    <t>5,4,3,2,1</t>
+    <t>italic</t>
+  </si>
+  <si>
+    <t>underline</t>
+  </si>
+  <si>
+    <t>5|4|3|2|1</t>
   </si>
 </sst>
 </file>
@@ -864,20 +869,20 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.453125" customWidth="1"/>
     <col min="2" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" customWidth="1"/>
-    <col min="8" max="8" width="15.42578125" customWidth="1"/>
-    <col min="9" max="9" width="11.5703125" customWidth="1"/>
-    <col min="12" max="12" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.5703125" customWidth="1"/>
+    <col min="5" max="5" width="15.1796875" customWidth="1"/>
+    <col min="6" max="6" width="13.54296875" customWidth="1"/>
+    <col min="7" max="7" width="12.7265625" customWidth="1"/>
+    <col min="8" max="8" width="15.453125" customWidth="1"/>
+    <col min="9" max="9" width="11.54296875" customWidth="1"/>
+    <col min="12" max="12" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -921,7 +926,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>10</v>
       </c>
@@ -978,16 +983,16 @@
       <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="22.7265625" customWidth="1"/>
+    <col min="4" max="4" width="18.7265625" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -1004,7 +1009,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -1018,7 +1023,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>27</v>
       </c>
@@ -1026,7 +1031,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -1050,12 +1055,12 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" customWidth="1"/>
+    <col min="1" max="1" width="24.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>110</v>
       </c>
@@ -1085,16 +1090,16 @@
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="14.7265625" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="17.26953125" customWidth="1"/>
+    <col min="4" max="4" width="14.26953125" customWidth="1"/>
+    <col min="5" max="5" width="13.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>49</v>
       </c>
@@ -1114,7 +1119,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1134,7 +1139,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1148,7 +1153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1159,7 +1164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1173,7 +1178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1193,17 +1198,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DD3CC7F-96FA-4722-9354-DA6065EED849}">
   <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="31.140625" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.1796875" customWidth="1"/>
+    <col min="2" max="2" width="9.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -1211,7 +1216,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>96</v>
       </c>
@@ -1219,7 +1224,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>95</v>
       </c>
@@ -1227,7 +1232,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>94</v>
       </c>
@@ -1235,7 +1240,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>75</v>
       </c>
@@ -1243,7 +1248,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>97</v>
       </c>
@@ -1251,7 +1256,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>98</v>
       </c>
@@ -1259,15 +1264,15 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>99</v>
       </c>
       <c r="B8" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>77</v>
       </c>
@@ -1275,7 +1280,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>134</v>
       </c>
@@ -1283,7 +1288,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>135</v>
       </c>
@@ -1291,15 +1296,15 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>136</v>
       </c>
       <c r="B12" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>137</v>
       </c>
@@ -1307,7 +1312,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>79</v>
       </c>
@@ -1315,7 +1320,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>80</v>
       </c>
@@ -1323,7 +1328,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>81</v>
       </c>
@@ -1331,7 +1336,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>82</v>
       </c>
@@ -1339,7 +1344,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>83</v>
       </c>
@@ -1347,7 +1352,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>85</v>
       </c>
@@ -1355,7 +1360,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>100</v>
       </c>
@@ -1363,7 +1368,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>87</v>
       </c>
@@ -1371,7 +1376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>88</v>
       </c>
@@ -1379,7 +1384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>89</v>
       </c>
@@ -1387,7 +1392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>90</v>
       </c>
@@ -1395,7 +1400,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>91</v>
       </c>
@@ -1403,7 +1408,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>101</v>
       </c>
@@ -1411,7 +1416,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>92</v>
       </c>
@@ -1419,7 +1424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>93</v>
       </c>
@@ -1440,24 +1445,24 @@
       <selection sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>48</v>
       </c>
@@ -1475,16 +1480,16 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" customWidth="1"/>
-    <col min="2" max="2" width="38.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1"/>
-    <col min="4" max="4" width="27.42578125" customWidth="1"/>
-    <col min="5" max="5" width="23.28515625" customWidth="1"/>
+    <col min="1" max="1" width="17.54296875" customWidth="1"/>
+    <col min="2" max="2" width="38.7265625" customWidth="1"/>
+    <col min="3" max="3" width="15.1796875" customWidth="1"/>
+    <col min="4" max="4" width="27.453125" customWidth="1"/>
+    <col min="5" max="5" width="23.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1501,7 +1506,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1518,7 +1523,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1535,7 +1540,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1565,9 +1570,9 @@
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>129</v>
       </c>
@@ -1585,9 +1590,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>129</v>
       </c>
@@ -1605,12 +1610,12 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" customWidth="1"/>
+    <col min="1" max="1" width="15.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>129</v>
       </c>
@@ -1618,7 +1623,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>70</v>
       </c>
@@ -1639,13 +1644,13 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="1" max="1" width="25.81640625" customWidth="1"/>
+    <col min="2" max="2" width="22.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>116</v>
       </c>
@@ -1653,7 +1658,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>120</v>
       </c>
@@ -1661,7 +1666,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>122</v>
       </c>
@@ -1669,7 +1674,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>124</v>
       </c>
@@ -1677,13 +1682,13 @@
         <v>125</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B7" s="2"/>
     </row>
   </sheetData>
@@ -1696,16 +1701,16 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="4" width="12.5703125" customWidth="1"/>
+    <col min="2" max="4" width="12.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -1725,7 +1730,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1733,7 +1738,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1741,12 +1746,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1754,7 +1759,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -1762,7 +1767,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -1770,7 +1775,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -1778,10 +1783,10 @@
         <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>138</v>
       </c>
@@ -1789,7 +1794,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -1797,7 +1802,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -1805,7 +1810,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -1813,7 +1818,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>138</v>
       </c>
@@ -1824,7 +1829,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -1832,7 +1837,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -1840,7 +1845,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -1848,7 +1853,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -1856,7 +1861,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -1864,7 +1869,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -1872,7 +1877,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -1880,7 +1885,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -1891,7 +1896,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -1899,7 +1904,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -1907,7 +1912,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -1928,9 +1933,9 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -1938,7 +1943,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1946,12 +1951,12 @@
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>116</v>
       </c>
@@ -1959,7 +1964,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>116</v>
       </c>
@@ -1967,7 +1972,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>116</v>
       </c>

</xml_diff>

<commit_message>
Handleiding digitoegankelijkheid geschreven, fout in weergeven aantallen opgelost, logo's toegevoegd aan digitoegankelijke versie.
</commit_message>
<xml_diff>
--- a/configuratie.xlsx
+++ b/configuratie.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hetservicecentrum-my.sharepoint.com/personal/a_dijkstra_ggdnog_nl/Documents/Documenten/Tabellenboek/GGData_tabellenboek/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="206" documentId="8_{0F18ABD2-A895-4412-9B00-D736EAC011EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{37B0C08A-1EA6-4E89-AE27-665A81CDEC4E}"/>
+  <xr:revisionPtr revIDLastSave="213" documentId="8_{0F18ABD2-A895-4412-9B00-D736EAC011EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{54A5AF69-2766-4DF6-A67D-187DFED7B119}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="7" activeTab="7" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="7" activeTab="10" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
   </bookViews>
   <sheets>
     <sheet name="algemeen" sheetId="5" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="153">
   <si>
     <t>naam_dataset</t>
   </si>
@@ -501,6 +501,12 @@
   </si>
   <si>
     <t>5|4|3|2|1</t>
+  </si>
+  <si>
+    <t>GGDNOG_logo.png</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -567,9 +573,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Thema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -607,7 +613,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -713,7 +719,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -855,7 +861,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1049,32 +1055,52 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B8BC91C-7A6C-4F7B-A16D-D5B583B31017}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.26953125" customWidth="1"/>
+    <col min="2" max="2" width="24.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B1" t="s">
         <v>110</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>111</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>112</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>113</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>-3</v>
+      </c>
+      <c r="E2">
+        <v>250</v>
+      </c>
+      <c r="F2">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1700,7 +1726,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6486BE4A-F285-45A5-8B7B-0E738AE5C353}">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Uitleg optie weergave toegevoegd aan handleiding en fout opgelost bij onderzoeksexport.
</commit_message>
<xml_diff>
--- a/configuratie.xlsx
+++ b/configuratie.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hetservicecentrum-my.sharepoint.com/personal/a_dijkstra_ggdnog_nl/Documents/Documenten/Tabellenboek/GGData_tabellenboek/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="213" documentId="8_{0F18ABD2-A895-4412-9B00-D736EAC011EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{54A5AF69-2766-4DF6-A67D-187DFED7B119}"/>
+  <xr:revisionPtr revIDLastSave="214" documentId="8_{0F18ABD2-A895-4412-9B00-D736EAC011EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C0281440-7455-4AE6-818D-39D5534198FC}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="7" activeTab="10" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
   </bookViews>
   <sheets>
     <sheet name="algemeen" sheetId="5" r:id="rId1"/>
@@ -446,9 +446,6 @@
     <t>weergave</t>
   </si>
   <si>
-    <t>n</t>
-  </si>
-  <si>
     <t>kolomkoppen</t>
   </si>
   <si>
@@ -507,6 +504,9 @@
   </si>
   <si>
     <t>id</t>
+  </si>
+  <si>
+    <t>perc</t>
   </si>
 </sst>
 </file>
@@ -871,24 +871,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB9555E0-3443-4710-AD14-3A977E907E6B}">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.453125" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
     <col min="2" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="15.1796875" customWidth="1"/>
-    <col min="6" max="6" width="13.54296875" customWidth="1"/>
-    <col min="7" max="7" width="12.7265625" customWidth="1"/>
-    <col min="8" max="8" width="15.453125" customWidth="1"/>
-    <col min="9" max="9" width="11.54296875" customWidth="1"/>
-    <col min="12" max="12" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.54296875" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" customWidth="1"/>
+    <col min="12" max="12" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -896,10 +896,10 @@
         <v>56</v>
       </c>
       <c r="C1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E1" t="s">
         <v>57</v>
@@ -926,13 +926,13 @@
         <v>128</v>
       </c>
       <c r="M1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>10</v>
       </c>
@@ -970,10 +970,10 @@
         <v>0</v>
       </c>
       <c r="M2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N2" t="s">
-        <v>132</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -989,16 +989,16 @@
       <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="22.7265625" customWidth="1"/>
-    <col min="4" max="4" width="18.7265625" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -1015,12 +1015,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1029,15 +1029,15 @@
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -1057,18 +1057,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B8BC91C-7A6C-4F7B-A16D-D5B583B31017}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="24.26953125" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B1" t="s">
         <v>110</v>
@@ -1086,9 +1086,9 @@
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C2">
         <v>3</v>
@@ -1116,16 +1116,16 @@
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.7265625" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="17.26953125" customWidth="1"/>
-    <col min="4" max="4" width="14.26953125" customWidth="1"/>
-    <col min="5" max="5" width="13.81640625" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>49</v>
       </c>
@@ -1145,7 +1145,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1165,7 +1165,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1179,7 +1179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1190,7 +1190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1204,7 +1204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1228,13 +1228,13 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.1796875" customWidth="1"/>
-    <col min="2" max="2" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.140625" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -1242,7 +1242,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>96</v>
       </c>
@@ -1250,7 +1250,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>95</v>
       </c>
@@ -1258,7 +1258,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>94</v>
       </c>
@@ -1266,7 +1266,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>75</v>
       </c>
@@ -1274,7 +1274,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>97</v>
       </c>
@@ -1282,7 +1282,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>98</v>
       </c>
@@ -1290,15 +1290,15 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>99</v>
       </c>
       <c r="B8" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>77</v>
       </c>
@@ -1306,39 +1306,39 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B10">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B11" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>135</v>
+      </c>
+      <c r="B12" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>136</v>
-      </c>
-      <c r="B12" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>137</v>
       </c>
       <c r="B13" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>79</v>
       </c>
@@ -1346,7 +1346,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>80</v>
       </c>
@@ -1354,7 +1354,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>81</v>
       </c>
@@ -1362,7 +1362,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>82</v>
       </c>
@@ -1370,7 +1370,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>83</v>
       </c>
@@ -1378,7 +1378,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>85</v>
       </c>
@@ -1386,7 +1386,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>100</v>
       </c>
@@ -1394,7 +1394,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>87</v>
       </c>
@@ -1402,7 +1402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>88</v>
       </c>
@@ -1410,7 +1410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>89</v>
       </c>
@@ -1418,7 +1418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>90</v>
       </c>
@@ -1426,15 +1426,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>91</v>
       </c>
       <c r="B25" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>101</v>
       </c>
@@ -1442,7 +1442,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>92</v>
       </c>
@@ -1450,7 +1450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>93</v>
       </c>
@@ -1471,24 +1471,24 @@
       <selection sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>48</v>
       </c>
@@ -1506,16 +1506,16 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.54296875" customWidth="1"/>
-    <col min="2" max="2" width="38.7265625" customWidth="1"/>
-    <col min="3" max="3" width="15.1796875" customWidth="1"/>
-    <col min="4" max="4" width="27.453125" customWidth="1"/>
-    <col min="5" max="5" width="23.26953125" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+    <col min="2" max="2" width="38.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1532,7 +1532,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1549,7 +1549,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1566,7 +1566,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1596,9 +1596,9 @@
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>129</v>
       </c>
@@ -1616,9 +1616,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>129</v>
       </c>
@@ -1636,12 +1636,12 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.81640625" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>129</v>
       </c>
@@ -1649,7 +1649,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>70</v>
       </c>
@@ -1670,13 +1670,13 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.81640625" customWidth="1"/>
-    <col min="2" max="2" width="22.1796875" customWidth="1"/>
+    <col min="1" max="1" width="25.85546875" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>116</v>
       </c>
@@ -1684,7 +1684,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>120</v>
       </c>
@@ -1692,7 +1692,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>122</v>
       </c>
@@ -1700,7 +1700,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>124</v>
       </c>
@@ -1708,13 +1708,13 @@
         <v>125</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
     </row>
   </sheetData>
@@ -1730,13 +1730,13 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="4" width="12.54296875" customWidth="1"/>
+    <col min="2" max="4" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -1744,10 +1744,10 @@
         <v>18</v>
       </c>
       <c r="C1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E1" t="s">
         <v>126</v>
@@ -1756,7 +1756,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1764,7 +1764,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1772,12 +1772,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1785,7 +1785,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -1793,7 +1793,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -1801,7 +1801,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -1809,18 +1809,18 @@
         <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -1828,7 +1828,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -1836,7 +1836,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -1844,18 +1844,18 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B13" t="s">
         <v>33</v>
       </c>
       <c r="D13" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -1863,7 +1863,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -1871,7 +1871,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -1879,7 +1879,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -1887,7 +1887,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -1895,7 +1895,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -1903,7 +1903,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -1911,7 +1911,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -1919,10 +1919,10 @@
         <v>41</v>
       </c>
       <c r="D21" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -1930,7 +1930,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -1938,7 +1938,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -1959,9 +1959,9 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -1969,7 +1969,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1977,12 +1977,12 @@
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>116</v>
       </c>
@@ -1990,7 +1990,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>116</v>
       </c>
@@ -1998,7 +1998,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>116</v>
       </c>

</xml_diff>

<commit_message>
Toegevoegd: - nvar is terug van weggeweest. - Title-element toegevoegd aan de digitoegankelijke versie, zodat significante resultaten daar ook leesbaar zijn voor screenreaders. Voor niet-screenreaders verschijnt dit als een tekstbubbel wanneer de muis erop staat. Hiervoor is een nieuwe instelling toegevoegd aan het tabblad algemeen.
Aangepast:
- Kleurschema afwisselende kolomkleuring aangepast in de digitoegankelijke versie, zodat deze overeenkomt met Excel.
- Om nvar mogelijk te maken zonder herberekening is de controle op eerdere resultaten aangepast. Dit zou verder niet merkbaar moeten zijn.
</commit_message>
<xml_diff>
--- a/configuratie.xlsx
+++ b/configuratie.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hetservicecentrum-my.sharepoint.com/personal/a_dijkstra_ggdnog_nl/Documents/Documenten/Tabellenboek/GGData_tabellenboek/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="214" documentId="8_{0F18ABD2-A895-4412-9B00-D736EAC011EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C0281440-7455-4AE6-818D-39D5534198FC}"/>
+  <xr:revisionPtr revIDLastSave="234" documentId="8_{0F18ABD2-A895-4412-9B00-D736EAC011EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{57941485-95C1-4DAE-AE64-8AE058E493A9}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="4" activeTab="7" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
   </bookViews>
   <sheets>
     <sheet name="algemeen" sheetId="5" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="158">
   <si>
     <t>naam_dataset</t>
   </si>
@@ -497,16 +497,31 @@
     <t>underline</t>
   </si>
   <si>
+    <t>GGDNOG_logo.png</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>perc</t>
+  </si>
+  <si>
+    <t>Een tekstregel, gevolgd door een lege regel:</t>
+  </si>
+  <si>
+    <t>En weer tekst!</t>
+  </si>
+  <si>
     <t>5|4|3|2|1</t>
   </si>
   <si>
-    <t>GGDNOG_logo.png</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>perc</t>
+    <t>nvar</t>
+  </si>
+  <si>
+    <t>sign_hovertekst</t>
+  </si>
+  <si>
+    <t>Deze waarde is significant anders.</t>
   </si>
 </sst>
 </file>
@@ -573,9 +588,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Thema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -613,7 +628,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -719,7 +734,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -861,7 +876,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -869,26 +884,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB9555E0-3443-4710-AD14-3A977E907E6B}">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.453125" customWidth="1"/>
     <col min="2" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" customWidth="1"/>
-    <col min="8" max="8" width="15.42578125" customWidth="1"/>
-    <col min="9" max="9" width="11.5703125" customWidth="1"/>
-    <col min="12" max="12" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.5703125" customWidth="1"/>
+    <col min="5" max="5" width="15.1796875" customWidth="1"/>
+    <col min="6" max="6" width="13.54296875" customWidth="1"/>
+    <col min="7" max="7" width="12.7265625" customWidth="1"/>
+    <col min="8" max="9" width="15.453125" customWidth="1"/>
+    <col min="10" max="10" width="11.54296875" customWidth="1"/>
+    <col min="13" max="13" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -914,25 +929,28 @@
         <v>60</v>
       </c>
       <c r="I1" t="s">
+        <v>156</v>
+      </c>
+      <c r="J1" t="s">
         <v>61</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>62</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>5</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>128</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>143</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>10</v>
       </c>
@@ -957,23 +975,26 @@
       <c r="H2" t="b">
         <v>1</v>
       </c>
-      <c r="I2">
+      <c r="I2" t="s">
+        <v>157</v>
+      </c>
+      <c r="J2">
         <v>0</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>0.01</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>8</v>
       </c>
-      <c r="L2" t="b">
+      <c r="M2" t="b">
         <v>0</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>144</v>
       </c>
-      <c r="N2" t="s">
-        <v>152</v>
+      <c r="O2" t="s">
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -989,16 +1010,16 @@
       <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="22.7265625" customWidth="1"/>
+    <col min="4" max="4" width="18.7265625" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -1015,7 +1036,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -1029,7 +1050,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>27</v>
       </c>
@@ -1037,7 +1058,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -1061,14 +1082,14 @@
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="24.28515625" customWidth="1"/>
+    <col min="2" max="2" width="24.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B1" t="s">
         <v>110</v>
@@ -1086,9 +1107,9 @@
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C2">
         <v>3</v>
@@ -1116,16 +1137,16 @@
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="14.7265625" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="17.26953125" customWidth="1"/>
+    <col min="4" max="4" width="14.26953125" customWidth="1"/>
+    <col min="5" max="5" width="13.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>49</v>
       </c>
@@ -1145,7 +1166,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1165,7 +1186,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1179,7 +1200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1190,7 +1211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1204,7 +1225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1228,13 +1249,13 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="31.140625" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.1796875" customWidth="1"/>
+    <col min="2" max="2" width="9.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -1242,7 +1263,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>96</v>
       </c>
@@ -1250,7 +1271,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>95</v>
       </c>
@@ -1258,7 +1279,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>94</v>
       </c>
@@ -1266,7 +1287,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>75</v>
       </c>
@@ -1274,7 +1295,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>97</v>
       </c>
@@ -1282,7 +1303,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>98</v>
       </c>
@@ -1290,7 +1311,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>99</v>
       </c>
@@ -1298,7 +1319,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>77</v>
       </c>
@@ -1306,7 +1327,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>133</v>
       </c>
@@ -1314,7 +1335,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>134</v>
       </c>
@@ -1322,7 +1343,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>135</v>
       </c>
@@ -1330,7 +1351,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>136</v>
       </c>
@@ -1338,7 +1359,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>79</v>
       </c>
@@ -1346,7 +1367,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>80</v>
       </c>
@@ -1354,7 +1375,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>81</v>
       </c>
@@ -1362,7 +1383,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>82</v>
       </c>
@@ -1370,7 +1391,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>83</v>
       </c>
@@ -1378,7 +1399,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>85</v>
       </c>
@@ -1386,7 +1407,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>100</v>
       </c>
@@ -1394,7 +1415,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>87</v>
       </c>
@@ -1402,7 +1423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>88</v>
       </c>
@@ -1410,7 +1431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>89</v>
       </c>
@@ -1418,7 +1439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>90</v>
       </c>
@@ -1426,7 +1447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>91</v>
       </c>
@@ -1434,7 +1455,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>101</v>
       </c>
@@ -1442,7 +1463,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>92</v>
       </c>
@@ -1450,7 +1471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>93</v>
       </c>
@@ -1471,24 +1492,24 @@
       <selection sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>48</v>
       </c>
@@ -1506,16 +1527,16 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" customWidth="1"/>
-    <col min="2" max="2" width="38.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1"/>
-    <col min="4" max="4" width="27.42578125" customWidth="1"/>
-    <col min="5" max="5" width="23.28515625" customWidth="1"/>
+    <col min="1" max="1" width="17.54296875" customWidth="1"/>
+    <col min="2" max="2" width="38.7265625" customWidth="1"/>
+    <col min="3" max="3" width="15.1796875" customWidth="1"/>
+    <col min="4" max="4" width="27.453125" customWidth="1"/>
+    <col min="5" max="5" width="23.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1532,7 +1553,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1549,7 +1570,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1566,7 +1587,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1596,9 +1617,9 @@
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>129</v>
       </c>
@@ -1616,9 +1637,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>129</v>
       </c>
@@ -1636,12 +1657,12 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" customWidth="1"/>
+    <col min="1" max="1" width="15.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>129</v>
       </c>
@@ -1649,7 +1670,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>70</v>
       </c>
@@ -1670,13 +1691,13 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="1" max="1" width="25.81640625" customWidth="1"/>
+    <col min="2" max="2" width="22.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>116</v>
       </c>
@@ -1684,7 +1705,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>120</v>
       </c>
@@ -1692,7 +1713,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>122</v>
       </c>
@@ -1700,7 +1721,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>124</v>
       </c>
@@ -1708,13 +1729,13 @@
         <v>125</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B7" s="2"/>
     </row>
   </sheetData>
@@ -1724,19 +1745,19 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6486BE4A-F285-45A5-8B7B-0E738AE5C353}">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="4" width="12.5703125" customWidth="1"/>
+    <col min="2" max="4" width="12.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -1756,7 +1777,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1764,7 +1785,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1772,12 +1793,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1785,7 +1806,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -1793,7 +1814,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -1801,18 +1822,18 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>155</v>
       </c>
       <c r="B8" t="s">
         <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>137</v>
       </c>
@@ -1820,7 +1841,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -1828,7 +1849,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -1836,7 +1857,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -1844,7 +1865,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>137</v>
       </c>
@@ -1855,94 +1876,115 @@
         <v>138</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>155</v>
       </c>
       <c r="B14" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>155</v>
       </c>
       <c r="B15" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>155</v>
       </c>
       <c r="B16" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>155</v>
       </c>
       <c r="B17" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
+        <v>116</v>
+      </c>
+      <c r="B18" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>116</v>
+      </c>
+      <c r="B20" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
         <v>19</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B21" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>26</v>
-      </c>
-      <c r="B19" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>26</v>
-      </c>
-      <c r="B21" t="s">
-        <v>41</v>
-      </c>
-      <c r="D21" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>26</v>
       </c>
       <c r="B22" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>26</v>
       </c>
       <c r="B24" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1959,9 +2001,9 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -1969,7 +2011,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1977,12 +2019,12 @@
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>116</v>
       </c>
@@ -1990,7 +2032,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>116</v>
       </c>
@@ -1998,7 +2040,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>116</v>
       </c>

</xml_diff>

<commit_message>
Mogelijkheid toegevoegd om zelf de naam in te stellen bij een tabellenboek zonder subset. (Was voorheen standaard 'Overzicht'.)
</commit_message>
<xml_diff>
--- a/configuratie.xlsx
+++ b/configuratie.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hetservicecentrum-my.sharepoint.com/personal/a_dijkstra_ggdnog_nl/Documents/Documenten/Tabellenboek/GGData_tabellenboek/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="234" documentId="8_{0F18ABD2-A895-4412-9B00-D736EAC011EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{57941485-95C1-4DAE-AE64-8AE058E493A9}"/>
+  <xr:revisionPtr revIDLastSave="236" documentId="8_{0F18ABD2-A895-4412-9B00-D736EAC011EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{99C3DBB4-DD7E-4422-B9BB-9674AEBA10DA}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="4" activeTab="7" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="9" activeTab="12" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
   </bookViews>
   <sheets>
     <sheet name="algemeen" sheetId="5" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="160">
   <si>
     <t>naam_dataset</t>
   </si>
@@ -522,6 +522,12 @@
   </si>
   <si>
     <t>Deze waarde is significant anders.</t>
+  </si>
+  <si>
+    <t>naam_tabellenboek</t>
+  </si>
+  <si>
+    <t>Overzicht</t>
   </si>
 </sst>
 </file>
@@ -1243,10 +1249,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DD3CC7F-96FA-4722-9354-DA6065EED849}">
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1477,6 +1483,14 @@
       </c>
       <c r="B28">
         <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>158</v>
+      </c>
+      <c r="B29" t="s">
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -1747,7 +1761,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6486BE4A-F285-45A5-8B7B-0E738AE5C353}">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Mogelijkheid toegevoegd om de weergave van significantie te verschuiven van de bronkolom naar de doelkolom.
</commit_message>
<xml_diff>
--- a/configuratie.xlsx
+++ b/configuratie.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hetservicecentrum-my.sharepoint.com/personal/a_dijkstra_ggdnog_nl/Documents/Documenten/Tabellenboek/GGData_tabellenboek/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="236" documentId="8_{0F18ABD2-A895-4412-9B00-D736EAC011EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{99C3DBB4-DD7E-4422-B9BB-9674AEBA10DA}"/>
+  <xr:revisionPtr revIDLastSave="239" documentId="8_{0F18ABD2-A895-4412-9B00-D736EAC011EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9526B192-83E8-4486-82F7-15F2E059474C}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="9" activeTab="12" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="9" activeTab="11" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
   </bookViews>
   <sheets>
     <sheet name="algemeen" sheetId="5" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="161">
   <si>
     <t>naam_dataset</t>
   </si>
@@ -528,6 +528,9 @@
   </si>
   <si>
     <t>Overzicht</t>
+  </si>
+  <si>
+    <t>sign_doelkolom</t>
   </si>
 </sst>
 </file>
@@ -896,20 +899,20 @@
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.453125" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
     <col min="2" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="15.1796875" customWidth="1"/>
-    <col min="6" max="6" width="13.54296875" customWidth="1"/>
-    <col min="7" max="7" width="12.7265625" customWidth="1"/>
-    <col min="8" max="9" width="15.453125" customWidth="1"/>
-    <col min="10" max="10" width="11.54296875" customWidth="1"/>
-    <col min="13" max="13" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.54296875" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="8" max="9" width="15.42578125" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" customWidth="1"/>
+    <col min="13" max="13" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -956,7 +959,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>10</v>
       </c>
@@ -1016,16 +1019,16 @@
       <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="22.7265625" customWidth="1"/>
-    <col min="4" max="4" width="18.7265625" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -1042,7 +1045,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -1056,7 +1059,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>27</v>
       </c>
@@ -1064,7 +1067,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -1088,12 +1091,12 @@
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="24.26953125" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>150</v>
       </c>
@@ -1113,7 +1116,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>149</v>
       </c>
@@ -1137,22 +1140,23 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C74130A8-7C80-4EF0-924A-78FEEA1CDE59}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.7265625" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="17.26953125" customWidth="1"/>
-    <col min="4" max="4" width="14.26953125" customWidth="1"/>
-    <col min="5" max="5" width="13.81640625" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>49</v>
       </c>
@@ -1171,8 +1175,11 @@
       <c r="F1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1191,8 +1198,11 @@
       <c r="F2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1206,7 +1216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1217,7 +1227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1231,7 +1241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1251,17 +1261,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DD3CC7F-96FA-4722-9354-DA6065EED849}">
   <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+    <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.1796875" customWidth="1"/>
-    <col min="2" max="2" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.140625" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -1269,7 +1279,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>96</v>
       </c>
@@ -1277,7 +1287,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>95</v>
       </c>
@@ -1285,7 +1295,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>94</v>
       </c>
@@ -1293,7 +1303,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>75</v>
       </c>
@@ -1301,7 +1311,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>97</v>
       </c>
@@ -1309,7 +1319,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>98</v>
       </c>
@@ -1317,7 +1327,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>99</v>
       </c>
@@ -1325,7 +1335,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>77</v>
       </c>
@@ -1333,7 +1343,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>133</v>
       </c>
@@ -1341,7 +1351,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>134</v>
       </c>
@@ -1349,7 +1359,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>135</v>
       </c>
@@ -1357,7 +1367,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>136</v>
       </c>
@@ -1365,7 +1375,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>79</v>
       </c>
@@ -1373,7 +1383,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>80</v>
       </c>
@@ -1381,7 +1391,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>81</v>
       </c>
@@ -1389,7 +1399,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>82</v>
       </c>
@@ -1397,7 +1407,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>83</v>
       </c>
@@ -1405,7 +1415,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>85</v>
       </c>
@@ -1413,7 +1423,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>100</v>
       </c>
@@ -1421,7 +1431,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>87</v>
       </c>
@@ -1429,7 +1439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>88</v>
       </c>
@@ -1437,7 +1447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>89</v>
       </c>
@@ -1445,7 +1455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>90</v>
       </c>
@@ -1453,7 +1463,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>91</v>
       </c>
@@ -1461,7 +1471,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>101</v>
       </c>
@@ -1469,7 +1479,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>92</v>
       </c>
@@ -1477,7 +1487,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>93</v>
       </c>
@@ -1485,7 +1495,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>158</v>
       </c>
@@ -1506,24 +1516,24 @@
       <selection sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>48</v>
       </c>
@@ -1541,16 +1551,16 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.54296875" customWidth="1"/>
-    <col min="2" max="2" width="38.7265625" customWidth="1"/>
-    <col min="3" max="3" width="15.1796875" customWidth="1"/>
-    <col min="4" max="4" width="27.453125" customWidth="1"/>
-    <col min="5" max="5" width="23.26953125" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+    <col min="2" max="2" width="38.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1567,7 +1577,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1584,7 +1594,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1601,7 +1611,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1631,9 +1641,9 @@
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>129</v>
       </c>
@@ -1651,9 +1661,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>129</v>
       </c>
@@ -1671,12 +1681,12 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.81640625" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>129</v>
       </c>
@@ -1684,7 +1694,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>70</v>
       </c>
@@ -1705,13 +1715,13 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.81640625" customWidth="1"/>
-    <col min="2" max="2" width="22.1796875" customWidth="1"/>
+    <col min="1" max="1" width="25.85546875" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>116</v>
       </c>
@@ -1719,7 +1729,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>120</v>
       </c>
@@ -1727,7 +1737,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>122</v>
       </c>
@@ -1735,7 +1745,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>124</v>
       </c>
@@ -1743,13 +1753,13 @@
         <v>125</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
     </row>
   </sheetData>
@@ -1765,13 +1775,13 @@
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="4" width="12.54296875" customWidth="1"/>
+    <col min="2" max="4" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -1791,7 +1801,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1799,7 +1809,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1807,12 +1817,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1820,7 +1830,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -1828,7 +1838,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -1836,7 +1846,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>155</v>
       </c>
@@ -1847,7 +1857,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>137</v>
       </c>
@@ -1855,7 +1865,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -1863,7 +1873,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -1871,7 +1881,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -1879,7 +1889,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>137</v>
       </c>
@@ -1890,7 +1900,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>155</v>
       </c>
@@ -1898,7 +1908,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>155</v>
       </c>
@@ -1906,7 +1916,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>155</v>
       </c>
@@ -1914,7 +1924,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>155</v>
       </c>
@@ -1922,7 +1932,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>116</v>
       </c>
@@ -1930,12 +1940,12 @@
         <v>152</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>116</v>
       </c>
@@ -1943,7 +1953,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1951,7 +1961,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -1959,7 +1969,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -1967,7 +1977,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -1978,7 +1988,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -1986,7 +1996,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -1994,7 +2004,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -2015,9 +2025,9 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -2025,7 +2035,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -2033,12 +2043,12 @@
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>116</v>
       </c>
@@ -2046,7 +2056,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>116</v>
       </c>
@@ -2054,7 +2064,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>116</v>
       </c>

</xml_diff>

<commit_message>
Naamgeving afgeleide datasets nu mogelijk. Uitgelegd in handleiding en basis config aangepast.
</commit_message>
<xml_diff>
--- a/configuratie.xlsx
+++ b/configuratie.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hetservicecentrum-my.sharepoint.com/personal/a_dijkstra_ggdnog_nl/Documents/Documenten/Tabellenboek/GGData_tabellenboek/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\Projecten\Project E-MOVO\2023\3 Uitvoering\Tabellenboeken\GGData_tabellenboek\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="239" documentId="8_{0F18ABD2-A895-4412-9B00-D736EAC011EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9526B192-83E8-4486-82F7-15F2E059474C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{599F2318-3328-4A84-ADFD-170B40F51004}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="9" activeTab="11" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
   </bookViews>
   <sheets>
     <sheet name="algemeen" sheetId="5" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="162">
   <si>
     <t>naam_dataset</t>
   </si>
@@ -531,6 +531,9 @@
   </si>
   <si>
     <t>sign_doelkolom</t>
+  </si>
+  <si>
+    <t>filter</t>
   </si>
 </sst>
 </file>
@@ -1142,7 +1145,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C74130A8-7C80-4EF0-924A-78FEEA1CDE59}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
@@ -1545,10 +1548,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27E157EC-B8A8-4DD4-B0B0-EC0F5BEAABD9}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1560,7 +1563,7 @@
     <col min="5" max="5" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1576,8 +1579,11 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1594,7 +1600,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1611,7 +1617,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Optie toegevoegd om enkel lege totaalkolommen of lege crossingkolommen te verbergen. Fout opgelost waarbij een subset met een enkele waarde (bijv. regio = GGD) zorgde voor het verdwijnen van de namen.
</commit_message>
<xml_diff>
--- a/configuratie.xlsx
+++ b/configuratie.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\Projecten\Project E-MOVO\2023\3 Uitvoering\Tabellenboeken\GGData_tabellenboek\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hetservicecentrum-my.sharepoint.com/personal/a_dijkstra_ggdnog_nl/Documents/Documenten/Tabellenboek/GGData_tabellenboek/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{599F2318-3328-4A84-ADFD-170B40F51004}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{599F2318-3328-4A84-ADFD-170B40F51004}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E2A3A7A-3996-424B-9605-2F25725E9C39}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="5" activeTab="12" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
   </bookViews>
   <sheets>
     <sheet name="algemeen" sheetId="5" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="164">
   <si>
     <t>naam_dataset</t>
   </si>
@@ -534,6 +534,12 @@
   </si>
   <si>
     <t>filter</t>
+  </si>
+  <si>
+    <t>verberg_lege_kolommen_crossing</t>
+  </si>
+  <si>
+    <t>verberg_lege_kolommen_totaal</t>
   </si>
 </sst>
 </file>
@@ -1262,10 +1268,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DD3CC7F-96FA-4722-9354-DA6065EED849}">
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1504,6 +1510,22 @@
       </c>
       <c r="B29" t="s">
         <v>159</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>162</v>
+      </c>
+      <c r="B30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>163</v>
+      </c>
+      <c r="B31" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1550,8 +1572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27E157EC-B8A8-4DD4-B0B0-EC0F5BEAABD9}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Mogelijkheid toegevoegd om het script te forceren om resultaten opnieuw te berekenen, ook al zijn er al resultaten bekend. Dit is bv handig als de data is veranderd.
</commit_message>
<xml_diff>
--- a/configuratie.xlsx
+++ b/configuratie.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hetservicecentrum-my.sharepoint.com/personal/a_dijkstra_ggdnog_nl/Documents/Documenten/Tabellenboek/GGData_tabellenboek/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\Projecten\Project E-MOVO\2023\3 Uitvoering\Tabellenboeken\GGData_tabellenboek\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{599F2318-3328-4A84-ADFD-170B40F51004}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E2A3A7A-3996-424B-9605-2F25725E9C39}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9FC532D-4477-466C-B7A6-0F69B196DB05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="5" activeTab="12" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
   </bookViews>
   <sheets>
     <sheet name="algemeen" sheetId="5" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="165">
   <si>
     <t>naam_dataset</t>
   </si>
@@ -540,6 +540,9 @@
   </si>
   <si>
     <t>verberg_lege_kolommen_totaal</t>
+  </si>
+  <si>
+    <t>forceer_berekening</t>
   </si>
 </sst>
 </file>
@@ -902,10 +905,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB9555E0-3443-4710-AD14-3A977E907E6B}">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -919,9 +922,10 @@
     <col min="10" max="10" width="11.5703125" customWidth="1"/>
     <col min="13" max="13" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15.5703125" customWidth="1"/>
+    <col min="16" max="16" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -967,8 +971,11 @@
       <c r="O1" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>10</v>
       </c>
@@ -1013,6 +1020,9 @@
       </c>
       <c r="O2" t="s">
         <v>151</v>
+      </c>
+      <c r="P2" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1270,8 +1280,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DD3CC7F-96FA-4722-9354-DA6065EED849}">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fouten opgelost: - Wanneer de eerste kolom van een crossing leeg was bleef de hele tabel achter in de berekening. - Plaatsing van logo's in de digitoegankelijke versie werkte niet als de kolom id niet in de configuratie stond.
Extra functies:
- {logo} kan nu ook in de introtekst geplaatst worden, zodat deze beter op de plek gezet kan worden.
- Naast [naam], voor de naam van het tabellenboek, kan nu ook [variabelenaam] voor de subsets gebruikt worden. Hiermee zou je bijvoorbeeld "[naam] in de regio [subregio]" in de introtekst kunnen zetten.
</commit_message>
<xml_diff>
--- a/configuratie.xlsx
+++ b/configuratie.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\Projecten\Project E-MOVO\2023\3 Uitvoering\Tabellenboeken\GGData_tabellenboek\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hetservicecentrum-my.sharepoint.com/personal/a_dijkstra_ggdnog_nl/Documents/Documenten/Tabellenboek/GGData_tabellenboek/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9FC532D-4477-466C-B7A6-0F69B196DB05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{F9FC532D-4477-466C-B7A6-0F69B196DB05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC36E9E2-6849-4542-BAF4-101C8096B9FB}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="4" activeTab="8" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
   </bookViews>
   <sheets>
     <sheet name="algemeen" sheetId="5" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="166">
   <si>
     <t>naam_dataset</t>
   </si>
@@ -401,9 +401,6 @@
     <t>tekst</t>
   </si>
   <si>
-    <t>Dit tabellenboek is een conceptversie.</t>
-  </si>
-  <si>
     <t>Iedere GGD kan dit tabellenboek zelf uitdraaien met een specifieke configuratie.</t>
   </si>
   <si>
@@ -543,6 +540,12 @@
   </si>
   <si>
     <t>forceer_berekening</t>
+  </si>
+  <si>
+    <t>Dit tabellenboek is een conceptversie. Je kunt [naam] gebruiken voor de hoofdsubset, of andere subsets aanduiden met [subsetnaam].</t>
+  </si>
+  <si>
+    <t>Je zou bijvoorbeeld de subregio aan kunnen geven met [subregio].</t>
   </si>
 </sst>
 </file>
@@ -907,7 +910,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB9555E0-3443-4710-AD14-3A977E907E6B}">
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
@@ -933,10 +936,10 @@
         <v>56</v>
       </c>
       <c r="C1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E1" t="s">
         <v>57</v>
@@ -951,7 +954,7 @@
         <v>60</v>
       </c>
       <c r="I1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J1" t="s">
         <v>61</v>
@@ -963,16 +966,16 @@
         <v>5</v>
       </c>
       <c r="M1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="O1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="P1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -1001,7 +1004,7 @@
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J2">
         <v>0</v>
@@ -1016,10 +1019,10 @@
         <v>0</v>
       </c>
       <c r="N2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="O2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="P2" t="b">
         <v>0</v>
@@ -1069,7 +1072,7 @@
         <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1083,7 +1086,7 @@
         <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1117,7 +1120,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B1" t="s">
         <v>110</v>
@@ -1137,7 +1140,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C2">
         <v>3</v>
@@ -1195,7 +1198,7 @@
         <v>68</v>
       </c>
       <c r="G1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1351,7 +1354,7 @@
         <v>99</v>
       </c>
       <c r="B8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1364,7 +1367,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B10">
         <v>14</v>
@@ -1372,7 +1375,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B11" t="s">
         <v>73</v>
@@ -1380,15 +1383,15 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B13" t="s">
         <v>78</v>
@@ -1487,7 +1490,7 @@
         <v>91</v>
       </c>
       <c r="B25" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -1516,15 +1519,15 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>157</v>
+      </c>
+      <c r="B29" t="s">
         <v>158</v>
-      </c>
-      <c r="B29" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B30" t="b">
         <v>0</v>
@@ -1532,7 +1535,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B31" t="b">
         <v>0</v>
@@ -1612,7 +1615,7 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1683,7 +1686,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -1703,7 +1706,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -1726,7 +1729,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B1" t="s">
         <v>17</v>
@@ -1737,7 +1740,7 @@
         <v>70</v>
       </c>
       <c r="B2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -1764,31 +1767,31 @@
         <v>116</v>
       </c>
       <c r="B1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2" t="s">
         <v>120</v>
-      </c>
-      <c r="B2" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B3" t="s">
         <v>122</v>
-      </c>
-      <c r="B3" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B4" t="s">
         <v>124</v>
-      </c>
-      <c r="B4" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1827,16 +1830,16 @@
         <v>18</v>
       </c>
       <c r="C1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F1" t="s">
         <v>126</v>
-      </c>
-      <c r="F1" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1886,18 +1889,18 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B8" t="s">
         <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B9" t="s">
         <v>29</v>
@@ -1929,18 +1932,18 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B13" t="s">
         <v>33</v>
       </c>
       <c r="D13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B14" t="s">
         <v>34</v>
@@ -1948,7 +1951,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B15" t="s">
         <v>35</v>
@@ -1956,7 +1959,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B16" t="s">
         <v>36</v>
@@ -1964,7 +1967,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B17" t="s">
         <v>37</v>
@@ -1975,7 +1978,7 @@
         <v>116</v>
       </c>
       <c r="B18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1988,7 +1991,7 @@
         <v>116</v>
       </c>
       <c r="B20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -2023,7 +2026,7 @@
         <v>41</v>
       </c>
       <c r="D24" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -2057,10 +2060,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B67183C1-66AD-4636-988C-6C4146A80519}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2091,7 +2094,7 @@
         <v>116</v>
       </c>
       <c r="B4" t="s">
-        <v>117</v>
+        <v>164</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2099,11 +2102,19 @@
         <v>116</v>
       </c>
       <c r="B5" t="s">
-        <v>118</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B6" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>116</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Optie toegevoegd om verschillen die na afronding gelijk lijken te verbergen.
</commit_message>
<xml_diff>
--- a/configuratie.xlsx
+++ b/configuratie.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hetservicecentrum-my.sharepoint.com/personal/a_dijkstra_ggdnog_nl/Documents/Documenten/Tabellenboek/GGData_tabellenboek/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{F9FC532D-4477-466C-B7A6-0F69B196DB05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC36E9E2-6849-4542-BAF4-101C8096B9FB}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{F9FC532D-4477-466C-B7A6-0F69B196DB05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE003BF5-B716-4A6C-AE79-AC00C516D870}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="4" activeTab="8" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
   </bookViews>
   <sheets>
     <sheet name="algemeen" sheetId="5" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="168">
   <si>
     <t>naam_dataset</t>
   </si>
@@ -546,6 +546,12 @@
   </si>
   <si>
     <t>Je zou bijvoorbeeld de subregio aan kunnen geven met [subregio].</t>
+  </si>
+  <si>
+    <t>hoger_is_beter</t>
+  </si>
+  <si>
+    <t>sign_verbergen_wanneer_afgerond_gelijk</t>
   </si>
 </sst>
 </file>
@@ -908,27 +914,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB9555E0-3443-4710-AD14-3A977E907E6B}">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.453125" customWidth="1"/>
     <col min="2" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" customWidth="1"/>
-    <col min="8" max="9" width="15.42578125" customWidth="1"/>
-    <col min="10" max="10" width="11.5703125" customWidth="1"/>
-    <col min="13" max="13" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.5703125" customWidth="1"/>
-    <col min="16" max="16" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.1796875" customWidth="1"/>
+    <col min="6" max="6" width="13.54296875" customWidth="1"/>
+    <col min="7" max="7" width="12.7265625" customWidth="1"/>
+    <col min="8" max="10" width="15.453125" customWidth="1"/>
+    <col min="11" max="11" width="11.54296875" customWidth="1"/>
+    <col min="14" max="14" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.54296875" customWidth="1"/>
+    <col min="17" max="17" width="9.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -957,28 +963,31 @@
         <v>155</v>
       </c>
       <c r="J1" t="s">
+        <v>167</v>
+      </c>
+      <c r="K1" t="s">
         <v>61</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>62</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>5</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>127</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>142</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>130</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>10</v>
       </c>
@@ -1006,25 +1015,28 @@
       <c r="I2" t="s">
         <v>156</v>
       </c>
-      <c r="J2">
+      <c r="J2" t="b">
         <v>0</v>
       </c>
       <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
         <v>0.01</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>8</v>
       </c>
-      <c r="M2" t="b">
+      <c r="N2" t="b">
         <v>0</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>143</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>150</v>
       </c>
-      <c r="P2" t="b">
+      <c r="Q2" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1041,16 +1053,16 @@
       <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="22.7265625" customWidth="1"/>
+    <col min="4" max="4" width="18.7265625" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -1067,7 +1079,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -1081,7 +1093,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>27</v>
       </c>
@@ -1089,7 +1101,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -1113,12 +1125,12 @@
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="24.28515625" customWidth="1"/>
+    <col min="2" max="2" width="24.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>149</v>
       </c>
@@ -1138,7 +1150,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>148</v>
       </c>
@@ -1168,17 +1180,17 @@
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="14.7265625" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.26953125" customWidth="1"/>
+    <col min="4" max="4" width="14.26953125" customWidth="1"/>
+    <col min="5" max="5" width="13.81640625" customWidth="1"/>
+    <col min="6" max="6" width="14.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>49</v>
       </c>
@@ -1201,7 +1213,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1224,7 +1236,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1238,7 +1250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1249,7 +1261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1263,7 +1275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1287,13 +1299,13 @@
       <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="31.140625" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.1796875" customWidth="1"/>
+    <col min="2" max="2" width="9.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -1301,7 +1313,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>96</v>
       </c>
@@ -1309,7 +1321,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>95</v>
       </c>
@@ -1317,7 +1329,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>94</v>
       </c>
@@ -1325,7 +1337,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>75</v>
       </c>
@@ -1333,7 +1345,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>97</v>
       </c>
@@ -1341,7 +1353,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>98</v>
       </c>
@@ -1349,7 +1361,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>99</v>
       </c>
@@ -1357,7 +1369,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>77</v>
       </c>
@@ -1365,7 +1377,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>132</v>
       </c>
@@ -1373,7 +1385,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>133</v>
       </c>
@@ -1381,7 +1393,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>134</v>
       </c>
@@ -1389,7 +1401,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>135</v>
       </c>
@@ -1397,7 +1409,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>79</v>
       </c>
@@ -1405,7 +1417,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>80</v>
       </c>
@@ -1413,7 +1425,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>81</v>
       </c>
@@ -1421,7 +1433,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>82</v>
       </c>
@@ -1429,7 +1441,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>83</v>
       </c>
@@ -1437,7 +1449,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>85</v>
       </c>
@@ -1445,7 +1457,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>100</v>
       </c>
@@ -1453,7 +1465,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>87</v>
       </c>
@@ -1461,7 +1473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>88</v>
       </c>
@@ -1469,7 +1481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>89</v>
       </c>
@@ -1477,7 +1489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>90</v>
       </c>
@@ -1485,7 +1497,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>91</v>
       </c>
@@ -1493,7 +1505,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>101</v>
       </c>
@@ -1501,7 +1513,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>92</v>
       </c>
@@ -1509,7 +1521,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>93</v>
       </c>
@@ -1517,7 +1529,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>157</v>
       </c>
@@ -1525,7 +1537,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>161</v>
       </c>
@@ -1533,7 +1545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>162</v>
       </c>
@@ -1554,24 +1566,24 @@
       <selection sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>48</v>
       </c>
@@ -1589,16 +1601,16 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" customWidth="1"/>
-    <col min="2" max="2" width="38.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1"/>
-    <col min="4" max="4" width="27.42578125" customWidth="1"/>
-    <col min="5" max="5" width="23.28515625" customWidth="1"/>
+    <col min="1" max="1" width="17.54296875" customWidth="1"/>
+    <col min="2" max="2" width="38.7265625" customWidth="1"/>
+    <col min="3" max="3" width="15.1796875" customWidth="1"/>
+    <col min="4" max="4" width="27.453125" customWidth="1"/>
+    <col min="5" max="5" width="23.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1618,7 +1630,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1635,7 +1647,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1652,7 +1664,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1682,9 +1694,9 @@
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>128</v>
       </c>
@@ -1702,9 +1714,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>128</v>
       </c>
@@ -1722,12 +1734,12 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" customWidth="1"/>
+    <col min="1" max="1" width="15.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>128</v>
       </c>
@@ -1735,7 +1747,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>70</v>
       </c>
@@ -1756,13 +1768,13 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="1" max="1" width="25.81640625" customWidth="1"/>
+    <col min="2" max="2" width="22.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>116</v>
       </c>
@@ -1770,7 +1782,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>119</v>
       </c>
@@ -1778,7 +1790,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>121</v>
       </c>
@@ -1786,7 +1798,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>123</v>
       </c>
@@ -1794,13 +1806,13 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B7" s="2"/>
     </row>
   </sheetData>
@@ -1810,19 +1822,19 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6486BE4A-F285-45A5-8B7B-0E738AE5C353}">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="4" width="12.5703125" customWidth="1"/>
+    <col min="2" max="5" width="12.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -1830,19 +1842,22 @@
         <v>18</v>
       </c>
       <c r="C1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D1" t="s">
         <v>145</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>131</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>125</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1850,7 +1865,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1858,12 +1873,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1871,7 +1886,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -1879,7 +1894,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -1887,18 +1902,18 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>154</v>
       </c>
       <c r="B8" t="s">
         <v>28</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>136</v>
       </c>
@@ -1906,42 +1921,51 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>26</v>
       </c>
       <c r="B10" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>26</v>
       </c>
       <c r="B11" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>26</v>
       </c>
       <c r="B12" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>136</v>
       </c>
       <c r="B13" t="s">
         <v>33</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>154</v>
       </c>
@@ -1949,7 +1973,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>154</v>
       </c>
@@ -1957,7 +1981,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>154</v>
       </c>
@@ -1965,7 +1989,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>154</v>
       </c>
@@ -1973,7 +1997,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>116</v>
       </c>
@@ -1981,12 +2005,12 @@
         <v>151</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>116</v>
       </c>
@@ -1994,7 +2018,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -2002,7 +2026,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -2010,7 +2034,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -2018,18 +2042,18 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>26</v>
       </c>
       <c r="B24" t="s">
         <v>41</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -2037,7 +2061,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -2045,7 +2069,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -2062,13 +2086,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B67183C1-66AD-4636-988C-6C4146A80519}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -2076,7 +2100,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -2084,12 +2108,12 @@
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>116</v>
       </c>
@@ -2097,7 +2121,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>116</v>
       </c>
@@ -2105,7 +2129,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>116</v>
       </c>
@@ -2113,7 +2137,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>116</v>
       </c>

</xml_diff>

<commit_message>
Voorbeeldconfiguratie aangepast om selectieve crossings te laten zien.
</commit_message>
<xml_diff>
--- a/configuratie.xlsx
+++ b/configuratie.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hetservicecentrum-my.sharepoint.com/personal/a_dijkstra_ggdnog_nl/Documents/Documenten/Tabellenboek/GGData_tabellenboek/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{F9FC532D-4477-466C-B7A6-0F69B196DB05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE003BF5-B716-4A6C-AE79-AC00C516D870}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="13_ncr:1_{F9FC532D-4477-466C-B7A6-0F69B196DB05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{29A33E61-D175-4FEF-9423-E9E1BD4CA46D}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
   </bookViews>
   <sheets>
     <sheet name="algemeen" sheetId="5" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="169">
   <si>
     <t>naam_dataset</t>
   </si>
@@ -548,10 +548,13 @@
     <t>Je zou bijvoorbeeld de subregio aan kunnen geven met [subregio].</t>
   </si>
   <si>
-    <t>hoger_is_beter</t>
-  </si>
-  <si>
     <t>sign_verbergen_wanneer_afgerond_gelijk</t>
+  </si>
+  <si>
+    <t>verberg_crossings</t>
+  </si>
+  <si>
+    <t>toetsen</t>
   </si>
 </sst>
 </file>
@@ -916,25 +919,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB9555E0-3443-4710-AD14-3A977E907E6B}">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.453125" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
     <col min="2" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="15.1796875" customWidth="1"/>
-    <col min="6" max="6" width="13.54296875" customWidth="1"/>
-    <col min="7" max="7" width="12.7265625" customWidth="1"/>
-    <col min="8" max="10" width="15.453125" customWidth="1"/>
-    <col min="11" max="11" width="11.54296875" customWidth="1"/>
-    <col min="14" max="14" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.54296875" customWidth="1"/>
-    <col min="17" max="17" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="8" max="10" width="15.42578125" customWidth="1"/>
+    <col min="11" max="11" width="11.5703125" customWidth="1"/>
+    <col min="14" max="14" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.5703125" customWidth="1"/>
+    <col min="17" max="17" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -963,7 +966,7 @@
         <v>155</v>
       </c>
       <c r="J1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="K1" t="s">
         <v>61</v>
@@ -987,7 +990,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>10</v>
       </c>
@@ -1050,19 +1053,19 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="22.7265625" customWidth="1"/>
-    <col min="4" max="4" width="18.7265625" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -1079,7 +1082,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -1093,7 +1096,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>27</v>
       </c>
@@ -1101,7 +1104,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -1125,12 +1128,12 @@
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="24.26953125" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>149</v>
       </c>
@@ -1150,7 +1153,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>148</v>
       </c>
@@ -1177,20 +1180,20 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.7265625" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="17.26953125" customWidth="1"/>
-    <col min="4" max="4" width="14.26953125" customWidth="1"/>
-    <col min="5" max="5" width="13.81640625" customWidth="1"/>
-    <col min="6" max="6" width="14.453125" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>49</v>
       </c>
@@ -1213,7 +1216,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1236,7 +1239,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1250,7 +1253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1261,7 +1264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1275,7 +1278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1299,13 +1302,13 @@
       <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.1796875" customWidth="1"/>
-    <col min="2" max="2" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.140625" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -1313,7 +1316,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>96</v>
       </c>
@@ -1321,7 +1324,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>95</v>
       </c>
@@ -1329,7 +1332,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>94</v>
       </c>
@@ -1337,7 +1340,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>75</v>
       </c>
@@ -1345,7 +1348,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>97</v>
       </c>
@@ -1353,7 +1356,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>98</v>
       </c>
@@ -1361,7 +1364,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>99</v>
       </c>
@@ -1369,7 +1372,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>77</v>
       </c>
@@ -1377,7 +1380,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>132</v>
       </c>
@@ -1385,7 +1388,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>133</v>
       </c>
@@ -1393,7 +1396,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>134</v>
       </c>
@@ -1401,7 +1404,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>135</v>
       </c>
@@ -1409,7 +1412,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>79</v>
       </c>
@@ -1417,7 +1420,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>80</v>
       </c>
@@ -1425,7 +1428,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>81</v>
       </c>
@@ -1433,7 +1436,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>82</v>
       </c>
@@ -1441,7 +1444,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>83</v>
       </c>
@@ -1449,7 +1452,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>85</v>
       </c>
@@ -1457,7 +1460,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>100</v>
       </c>
@@ -1465,7 +1468,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>87</v>
       </c>
@@ -1473,7 +1476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>88</v>
       </c>
@@ -1481,7 +1484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>89</v>
       </c>
@@ -1489,7 +1492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>90</v>
       </c>
@@ -1497,7 +1500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>91</v>
       </c>
@@ -1505,7 +1508,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>101</v>
       </c>
@@ -1513,7 +1516,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>92</v>
       </c>
@@ -1521,7 +1524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>93</v>
       </c>
@@ -1529,7 +1532,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>157</v>
       </c>
@@ -1537,7 +1540,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>161</v>
       </c>
@@ -1545,7 +1548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>162</v>
       </c>
@@ -1560,32 +1563,47 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21FFED35-A9FD-48DB-B137-EE60E86B3C7B}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>48</v>
+      </c>
+      <c r="B4" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1601,16 +1619,16 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.54296875" customWidth="1"/>
-    <col min="2" max="2" width="38.7265625" customWidth="1"/>
-    <col min="3" max="3" width="15.1796875" customWidth="1"/>
-    <col min="4" max="4" width="27.453125" customWidth="1"/>
-    <col min="5" max="5" width="23.26953125" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+    <col min="2" max="2" width="38.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1630,7 +1648,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1647,7 +1665,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1664,7 +1682,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1694,9 +1712,9 @@
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>128</v>
       </c>
@@ -1714,9 +1732,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>128</v>
       </c>
@@ -1734,12 +1752,12 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.81640625" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>128</v>
       </c>
@@ -1747,7 +1765,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>70</v>
       </c>
@@ -1765,16 +1783,16 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.81640625" customWidth="1"/>
-    <col min="2" max="2" width="22.1796875" customWidth="1"/>
+    <col min="1" max="1" width="25.85546875" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>116</v>
       </c>
@@ -1782,7 +1800,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>119</v>
       </c>
@@ -1790,7 +1808,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>121</v>
       </c>
@@ -1798,7 +1816,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>123</v>
       </c>
@@ -1806,13 +1824,13 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
     </row>
   </sheetData>
@@ -1825,16 +1843,16 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="5" width="12.54296875" customWidth="1"/>
+    <col min="2" max="5" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -1842,13 +1860,13 @@
         <v>18</v>
       </c>
       <c r="C1" t="s">
-        <v>166</v>
+        <v>145</v>
       </c>
       <c r="D1" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="E1" t="s">
-        <v>131</v>
+        <v>167</v>
       </c>
       <c r="F1" t="s">
         <v>125</v>
@@ -1857,7 +1875,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1865,7 +1883,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1873,12 +1891,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1886,7 +1904,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -1894,26 +1912,29 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>26</v>
       </c>
       <c r="B7" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>154</v>
       </c>
       <c r="B8" t="s">
         <v>28</v>
       </c>
-      <c r="D8" t="s">
+      <c r="C8" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>136</v>
       </c>
@@ -1921,51 +1942,42 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>26</v>
       </c>
       <c r="B10" t="s">
         <v>30</v>
       </c>
-      <c r="C10" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>26</v>
       </c>
       <c r="B11" t="s">
         <v>31</v>
       </c>
-      <c r="C11" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>26</v>
       </c>
       <c r="B12" t="s">
         <v>32</v>
       </c>
-      <c r="C12" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>136</v>
       </c>
       <c r="B13" t="s">
         <v>33</v>
       </c>
-      <c r="E13" t="s">
+      <c r="D13" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>154</v>
       </c>
@@ -1973,7 +1985,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>154</v>
       </c>
@@ -1981,7 +1993,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>154</v>
       </c>
@@ -1989,7 +2001,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>154</v>
       </c>
@@ -1997,7 +2009,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>116</v>
       </c>
@@ -2005,12 +2017,12 @@
         <v>151</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>116</v>
       </c>
@@ -2018,7 +2030,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -2026,7 +2038,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -2034,7 +2046,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -2042,18 +2054,18 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>26</v>
       </c>
       <c r="B24" t="s">
         <v>41</v>
       </c>
-      <c r="E24" t="s">
+      <c r="D24" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -2061,7 +2073,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -2069,7 +2081,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -2090,9 +2102,9 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -2100,7 +2112,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -2108,12 +2120,12 @@
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>116</v>
       </c>
@@ -2121,7 +2133,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>116</v>
       </c>
@@ -2129,7 +2141,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>116</v>
       </c>
@@ -2137,7 +2149,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>116</v>
       </c>

</xml_diff>

<commit_message>
Multiple testing correction verplaatst naar na de berekening, zodat er niet per ongeluk een verkeerde correctie wordt uitgevoerd.
</commit_message>
<xml_diff>
--- a/configuratie.xlsx
+++ b/configuratie.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hetservicecentrum-my.sharepoint.com/personal/a_dijkstra_ggdnog_nl/Documents/Documenten/Tabellenboek/GGData_tabellenboek/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="35" documentId="13_ncr:1_{F9FC532D-4477-466C-B7A6-0F69B196DB05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{29A33E61-D175-4FEF-9423-E9E1BD4CA46D}"/>
+  <xr:revisionPtr revIDLastSave="38" documentId="13_ncr:1_{F9FC532D-4477-466C-B7A6-0F69B196DB05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F916EE56-0AEF-42AA-8651-D3EDFABD3592}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
   </bookViews>
   <sheets>
     <sheet name="algemeen" sheetId="5" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="171">
   <si>
     <t>naam_dataset</t>
   </si>
@@ -555,6 +555,12 @@
   </si>
   <si>
     <t>toetsen</t>
+  </si>
+  <si>
+    <t>multiple_testing_correction</t>
+  </si>
+  <si>
+    <t>BH</t>
   </si>
 </sst>
 </file>
@@ -917,10 +923,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB9555E0-3443-4710-AD14-3A977E907E6B}">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -930,14 +936,14 @@
     <col min="5" max="5" width="15.140625" customWidth="1"/>
     <col min="6" max="6" width="13.5703125" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" customWidth="1"/>
-    <col min="8" max="10" width="15.42578125" customWidth="1"/>
-    <col min="11" max="11" width="11.5703125" customWidth="1"/>
-    <col min="14" max="14" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.5703125" customWidth="1"/>
-    <col min="17" max="17" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="15.42578125" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" customWidth="1"/>
+    <col min="15" max="15" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.5703125" customWidth="1"/>
+    <col min="18" max="18" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -963,34 +969,37 @@
         <v>60</v>
       </c>
       <c r="I1" t="s">
+        <v>169</v>
+      </c>
+      <c r="J1" t="s">
         <v>155</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>166</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>61</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>62</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>5</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>127</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>142</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>130</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>10</v>
       </c>
@@ -1016,30 +1025,33 @@
         <v>1</v>
       </c>
       <c r="I2" t="s">
+        <v>170</v>
+      </c>
+      <c r="J2" t="s">
         <v>156</v>
       </c>
-      <c r="J2" t="b">
+      <c r="K2" t="b">
         <v>0</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>0</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>0.01</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>8</v>
       </c>
-      <c r="N2" t="b">
+      <c r="O2" t="b">
         <v>0</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>143</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>150</v>
       </c>
-      <c r="Q2" t="b">
+      <c r="R2" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1298,8 +1310,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DD3CC7F-96FA-4722-9354-DA6065EED849}">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1565,7 +1577,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21FFED35-A9FD-48DB-B137-EE60E86B3C7B}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Logica multiple testing correction aangepast zodat toetsen niet dubbel gerekend worden.
</commit_message>
<xml_diff>
--- a/configuratie.xlsx
+++ b/configuratie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hetservicecentrum-my.sharepoint.com/personal/a_dijkstra_ggdnog_nl/Documents/Documenten/Tabellenboek/GGData_tabellenboek/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="38" documentId="13_ncr:1_{F9FC532D-4477-466C-B7A6-0F69B196DB05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F916EE56-0AEF-42AA-8651-D3EDFABD3592}"/>
+  <xr:revisionPtr revIDLastSave="39" documentId="13_ncr:1_{F9FC532D-4477-466C-B7A6-0F69B196DB05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C1CC452C-7172-4EA0-8B53-CFDA74A2F23A}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
   </bookViews>
@@ -926,7 +926,7 @@
   <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1037,7 +1037,7 @@
         <v>0</v>
       </c>
       <c r="M2">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
       <c r="N2" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
standaardinstellingen vb excel veranderd. kleine herstructurering van de mtc code.
</commit_message>
<xml_diff>
--- a/configuratie.xlsx
+++ b/configuratie.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hetservicecentrum-my.sharepoint.com/personal/a_dijkstra_ggdnog_nl/Documents/Documenten/Tabellenboek/GGData_tabellenboek/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Repositories\GGData_tabellenboek\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="13_ncr:1_{F9FC532D-4477-466C-B7A6-0F69B196DB05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C1CC452C-7172-4EA0-8B53-CFDA74A2F23A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FA09F30-D5ED-4EB1-97AF-F71B471E06D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
   </bookViews>
   <sheets>
     <sheet name="algemeen" sheetId="5" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="174">
   <si>
     <t>naam_dataset</t>
   </si>
@@ -561,16 +561,32 @@
   </si>
   <si>
     <t>BH</t>
+  </si>
+  <si>
+    <t>aantal_toetsen</t>
+  </si>
+  <si>
+    <t>bonferroni</t>
+  </si>
+  <si>
+    <t>fpc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -601,7 +617,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -609,6 +625,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -923,10 +940,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB9555E0-3443-4710-AD14-3A977E907E6B}">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -943,7 +960,7 @@
     <col min="18" max="18" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -998,8 +1015,14 @@
       <c r="R1" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S1" t="s">
+        <v>169</v>
+      </c>
+      <c r="T1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>10</v>
       </c>
@@ -1054,6 +1077,10 @@
       <c r="R2" t="b">
         <v>0</v>
       </c>
+      <c r="S2" t="s">
+        <v>172</v>
+      </c>
+      <c r="T2" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1625,10 +1652,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27E157EC-B8A8-4DD4-B0B0-EC0F5BEAABD9}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1640,7 +1667,7 @@
     <col min="5" max="5" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1659,8 +1686,11 @@
       <c r="F1" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1677,7 +1707,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1694,7 +1724,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
multiple_testing_correction stond 2x in de sheet
</commit_message>
<xml_diff>
--- a/configuratie.xlsx
+++ b/configuratie.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Repositories\GGData_tabellenboek\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hetservicecentrum-my.sharepoint.com/personal/a_dijkstra_ggdnog_nl/Documents/Documenten/Tabellenboek/GGData_tabellenboek/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FA09F30-D5ED-4EB1-97AF-F71B471E06D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{6FA09F30-D5ED-4EB1-97AF-F71B471E06D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{63DAF61C-B4BF-4685-BCD4-06FA63A9FFF4}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
   </bookViews>
   <sheets>
     <sheet name="algemeen" sheetId="5" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="173">
   <si>
     <t>naam_dataset</t>
   </si>
@@ -558,9 +558,6 @@
   </si>
   <si>
     <t>multiple_testing_correction</t>
-  </si>
-  <si>
-    <t>BH</t>
   </si>
   <si>
     <t>aantal_toetsen</t>
@@ -940,27 +937,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB9555E0-3443-4710-AD14-3A977E907E6B}">
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="S6" sqref="S6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" customWidth="1"/>
     <col min="2" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" customWidth="1"/>
-    <col min="8" max="11" width="15.42578125" customWidth="1"/>
-    <col min="12" max="12" width="11.5703125" customWidth="1"/>
-    <col min="15" max="15" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.5703125" customWidth="1"/>
-    <col min="18" max="18" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" customWidth="1"/>
+    <col min="6" max="6" width="13.5546875" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" customWidth="1"/>
+    <col min="8" max="10" width="15.44140625" customWidth="1"/>
+    <col min="11" max="11" width="11.5546875" customWidth="1"/>
+    <col min="14" max="14" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.5546875" customWidth="1"/>
+    <col min="17" max="17" width="9.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -986,43 +983,40 @@
         <v>60</v>
       </c>
       <c r="I1" t="s">
+        <v>155</v>
+      </c>
+      <c r="J1" t="s">
+        <v>166</v>
+      </c>
+      <c r="K1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" t="s">
+        <v>127</v>
+      </c>
+      <c r="O1" t="s">
+        <v>142</v>
+      </c>
+      <c r="P1" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>163</v>
+      </c>
+      <c r="R1" t="s">
         <v>169</v>
       </c>
-      <c r="J1" t="s">
-        <v>155</v>
-      </c>
-      <c r="K1" t="s">
-        <v>166</v>
-      </c>
-      <c r="L1" t="s">
-        <v>61</v>
-      </c>
-      <c r="M1" t="s">
-        <v>62</v>
-      </c>
-      <c r="N1" t="s">
-        <v>5</v>
-      </c>
-      <c r="O1" t="s">
-        <v>127</v>
-      </c>
-      <c r="P1" t="s">
-        <v>142</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>130</v>
-      </c>
-      <c r="R1" t="s">
-        <v>163</v>
-      </c>
       <c r="S1" t="s">
-        <v>169</v>
-      </c>
-      <c r="T1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>10</v>
       </c>
@@ -1048,39 +1042,36 @@
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>170</v>
-      </c>
-      <c r="J2" t="s">
         <v>156</v>
       </c>
-      <c r="K2" t="b">
+      <c r="J2" t="b">
         <v>0</v>
       </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
       <c r="L2">
+        <v>0.05</v>
+      </c>
+      <c r="M2" t="s">
+        <v>8</v>
+      </c>
+      <c r="N2" t="b">
         <v>0</v>
       </c>
-      <c r="M2">
-        <v>0.05</v>
-      </c>
-      <c r="N2" t="s">
-        <v>8</v>
-      </c>
-      <c r="O2" t="b">
+      <c r="O2" t="s">
+        <v>143</v>
+      </c>
+      <c r="P2" t="s">
+        <v>150</v>
+      </c>
+      <c r="Q2" t="b">
         <v>0</v>
       </c>
-      <c r="P2" t="s">
-        <v>143</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>150</v>
-      </c>
-      <c r="R2" t="b">
-        <v>0</v>
-      </c>
-      <c r="S2" t="s">
-        <v>172</v>
-      </c>
-      <c r="T2" s="3"/>
+      <c r="R2" t="s">
+        <v>171</v>
+      </c>
+      <c r="S2" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1095,16 +1086,16 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -1121,7 +1112,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -1135,7 +1126,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>27</v>
       </c>
@@ -1143,7 +1134,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -1167,12 +1158,12 @@
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="24.28515625" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>149</v>
       </c>
@@ -1192,7 +1183,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>148</v>
       </c>
@@ -1222,17 +1213,17 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" customWidth="1"/>
+    <col min="6" max="6" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>49</v>
       </c>
@@ -1255,7 +1246,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1278,7 +1269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1292,7 +1283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1303,7 +1294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1317,7 +1308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1341,13 +1332,13 @@
       <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.140625" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.109375" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -1355,7 +1346,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>96</v>
       </c>
@@ -1363,7 +1354,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>95</v>
       </c>
@@ -1371,7 +1362,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>94</v>
       </c>
@@ -1379,7 +1370,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>75</v>
       </c>
@@ -1387,7 +1378,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>97</v>
       </c>
@@ -1395,7 +1386,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>98</v>
       </c>
@@ -1403,7 +1394,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>99</v>
       </c>
@@ -1411,7 +1402,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>77</v>
       </c>
@@ -1419,7 +1410,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>132</v>
       </c>
@@ -1427,7 +1418,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>133</v>
       </c>
@@ -1435,7 +1426,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>134</v>
       </c>
@@ -1443,7 +1434,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>135</v>
       </c>
@@ -1451,7 +1442,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>79</v>
       </c>
@@ -1459,7 +1450,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>80</v>
       </c>
@@ -1467,7 +1458,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>81</v>
       </c>
@@ -1475,7 +1466,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>82</v>
       </c>
@@ -1483,7 +1474,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>83</v>
       </c>
@@ -1491,7 +1482,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>85</v>
       </c>
@@ -1499,7 +1490,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>100</v>
       </c>
@@ -1507,7 +1498,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>87</v>
       </c>
@@ -1515,7 +1506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>88</v>
       </c>
@@ -1523,7 +1514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>89</v>
       </c>
@@ -1531,7 +1522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>90</v>
       </c>
@@ -1539,7 +1530,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>91</v>
       </c>
@@ -1547,7 +1538,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>101</v>
       </c>
@@ -1555,7 +1546,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>92</v>
       </c>
@@ -1563,7 +1554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>93</v>
       </c>
@@ -1571,7 +1562,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>157</v>
       </c>
@@ -1579,7 +1570,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>161</v>
       </c>
@@ -1587,7 +1578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>162</v>
       </c>
@@ -1608,12 +1599,12 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>45</v>
       </c>
@@ -1621,7 +1612,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>46</v>
       </c>
@@ -1629,7 +1620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>47</v>
       </c>
@@ -1637,7 +1628,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>48</v>
       </c>
@@ -1654,20 +1645,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27E157EC-B8A8-4DD4-B0B0-EC0F5BEAABD9}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" customWidth="1"/>
-    <col min="2" max="2" width="38.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1"/>
-    <col min="4" max="4" width="27.42578125" customWidth="1"/>
-    <col min="5" max="5" width="23.28515625" customWidth="1"/>
+    <col min="1" max="1" width="17.5546875" customWidth="1"/>
+    <col min="2" max="2" width="38.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" customWidth="1"/>
+    <col min="4" max="4" width="27.44140625" customWidth="1"/>
+    <col min="5" max="5" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1687,10 +1678,10 @@
         <v>160</v>
       </c>
       <c r="G1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1707,7 +1698,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1724,7 +1715,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1754,9 +1745,9 @@
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>128</v>
       </c>
@@ -1774,9 +1765,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>128</v>
       </c>
@@ -1794,12 +1785,12 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" customWidth="1"/>
+    <col min="1" max="1" width="15.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>128</v>
       </c>
@@ -1807,7 +1798,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>70</v>
       </c>
@@ -1828,13 +1819,13 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="1" max="1" width="25.88671875" customWidth="1"/>
+    <col min="2" max="2" width="22.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>116</v>
       </c>
@@ -1842,7 +1833,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>119</v>
       </c>
@@ -1850,7 +1841,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>121</v>
       </c>
@@ -1858,7 +1849,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>123</v>
       </c>
@@ -1866,13 +1857,13 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B7" s="2"/>
     </row>
   </sheetData>
@@ -1888,13 +1879,13 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="5" width="12.5703125" customWidth="1"/>
+    <col min="2" max="5" width="12.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -1917,7 +1908,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1925,7 +1916,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1933,12 +1924,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1946,7 +1937,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -1954,7 +1945,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -1965,7 +1956,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>154</v>
       </c>
@@ -1976,7 +1967,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>136</v>
       </c>
@@ -1984,7 +1975,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -1992,7 +1983,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -2000,7 +1991,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -2008,7 +1999,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>136</v>
       </c>
@@ -2019,7 +2010,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>154</v>
       </c>
@@ -2027,7 +2018,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>154</v>
       </c>
@@ -2035,7 +2026,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>154</v>
       </c>
@@ -2043,7 +2034,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>154</v>
       </c>
@@ -2051,7 +2042,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>116</v>
       </c>
@@ -2059,12 +2050,12 @@
         <v>151</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>116</v>
       </c>
@@ -2072,7 +2063,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -2080,7 +2071,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -2088,7 +2079,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -2096,7 +2087,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -2107,7 +2098,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -2115,7 +2106,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -2123,7 +2114,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -2144,9 +2135,9 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -2154,7 +2145,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -2162,12 +2153,12 @@
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>116</v>
       </c>
@@ -2175,7 +2166,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>116</v>
       </c>
@@ -2183,7 +2174,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>116</v>
       </c>
@@ -2191,7 +2182,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>116</v>
       </c>
@@ -2199,4 +2190,10 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{b4bf6224-2c81-4ea6-976b-a3e2a0d992db}" enabled="1" method="Standard" siteId="{6485e4ee-e92a-48ea-83c4-0d404781e21f}" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
Optie ingebouwd om middels benader_chisq in tabblad algemeen Rao–Scott first order design correctie toe te passen bij svychisq als Rao–Scott second order faalt door te kleine within-strata variantie. Dit is minder precies maar robuuster.
</commit_message>
<xml_diff>
--- a/configuratie.xlsx
+++ b/configuratie.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hetservicecentrum-my.sharepoint.com/personal/a_dijkstra_ggdnog_nl/Documents/Documenten/Tabellenboek/GGData_tabellenboek/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Repositories\GGData_tabellenboek\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{6FA09F30-D5ED-4EB1-97AF-F71B471E06D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{63DAF61C-B4BF-4685-BCD4-06FA63A9FFF4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BE4A256-B021-4485-A8EE-566368964380}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{ECC980AC-D294-4808-BCB8-F5A87956E45F}"/>
   </bookViews>
   <sheets>
     <sheet name="algemeen" sheetId="5" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="174">
   <si>
     <t>naam_dataset</t>
   </si>
@@ -567,6 +567,9 @@
   </si>
   <si>
     <t>fpc</t>
+  </si>
+  <si>
+    <t>benader_chisq</t>
   </si>
 </sst>
 </file>
@@ -937,27 +940,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB9555E0-3443-4710-AD14-3A977E907E6B}">
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
     <col min="2" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="15.109375" customWidth="1"/>
-    <col min="6" max="6" width="13.5546875" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" customWidth="1"/>
-    <col min="8" max="10" width="15.44140625" customWidth="1"/>
-    <col min="11" max="11" width="11.5546875" customWidth="1"/>
-    <col min="14" max="14" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.5546875" customWidth="1"/>
-    <col min="17" max="17" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="8" max="10" width="15.42578125" customWidth="1"/>
+    <col min="11" max="11" width="11.5703125" customWidth="1"/>
+    <col min="14" max="14" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.5703125" customWidth="1"/>
+    <col min="17" max="17" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -1015,8 +1019,11 @@
       <c r="S1" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>10</v>
       </c>
@@ -1072,6 +1079,9 @@
         <v>171</v>
       </c>
       <c r="S2" s="3"/>
+      <c r="T2" t="b">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1086,16 +1096,16 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="22.6640625" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -1112,7 +1122,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -1126,7 +1136,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>27</v>
       </c>
@@ -1134,7 +1144,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -1158,12 +1168,12 @@
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="24.33203125" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>149</v>
       </c>
@@ -1183,7 +1193,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>148</v>
       </c>
@@ -1213,17 +1223,17 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" customWidth="1"/>
-    <col min="5" max="5" width="13.88671875" customWidth="1"/>
-    <col min="6" max="6" width="14.44140625" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>49</v>
       </c>
@@ -1246,7 +1256,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1269,7 +1279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1283,7 +1293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1294,7 +1304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1308,7 +1318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1332,13 +1342,13 @@
       <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.109375" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.140625" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -1346,7 +1356,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>96</v>
       </c>
@@ -1354,7 +1364,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>95</v>
       </c>
@@ -1362,7 +1372,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>94</v>
       </c>
@@ -1370,7 +1380,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>75</v>
       </c>
@@ -1378,7 +1388,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>97</v>
       </c>
@@ -1386,7 +1396,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>98</v>
       </c>
@@ -1394,7 +1404,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>99</v>
       </c>
@@ -1402,7 +1412,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>77</v>
       </c>
@@ -1410,7 +1420,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>132</v>
       </c>
@@ -1418,7 +1428,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>133</v>
       </c>
@@ -1426,7 +1436,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>134</v>
       </c>
@@ -1434,7 +1444,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>135</v>
       </c>
@@ -1442,7 +1452,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>79</v>
       </c>
@@ -1450,7 +1460,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>80</v>
       </c>
@@ -1458,7 +1468,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>81</v>
       </c>
@@ -1466,7 +1476,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>82</v>
       </c>
@@ -1474,7 +1484,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>83</v>
       </c>
@@ -1482,7 +1492,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>85</v>
       </c>
@@ -1490,7 +1500,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>100</v>
       </c>
@@ -1498,7 +1508,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>87</v>
       </c>
@@ -1506,7 +1516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>88</v>
       </c>
@@ -1514,7 +1524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>89</v>
       </c>
@@ -1522,7 +1532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>90</v>
       </c>
@@ -1530,7 +1540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>91</v>
       </c>
@@ -1538,7 +1548,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>101</v>
       </c>
@@ -1546,7 +1556,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>92</v>
       </c>
@@ -1554,7 +1564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>93</v>
       </c>
@@ -1562,7 +1572,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>157</v>
       </c>
@@ -1570,7 +1580,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>161</v>
       </c>
@@ -1578,7 +1588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>162</v>
       </c>
@@ -1599,12 +1609,12 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>45</v>
       </c>
@@ -1612,7 +1622,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>46</v>
       </c>
@@ -1620,7 +1630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>47</v>
       </c>
@@ -1628,7 +1638,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>48</v>
       </c>
@@ -1649,16 +1659,16 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5546875" customWidth="1"/>
-    <col min="2" max="2" width="38.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.109375" customWidth="1"/>
-    <col min="4" max="4" width="27.44140625" customWidth="1"/>
-    <col min="5" max="5" width="23.33203125" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+    <col min="2" max="2" width="38.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1681,7 +1691,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1698,7 +1708,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1715,7 +1725,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1745,9 +1755,9 @@
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>128</v>
       </c>
@@ -1765,9 +1775,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>128</v>
       </c>
@@ -1785,12 +1795,12 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.88671875" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>128</v>
       </c>
@@ -1798,7 +1808,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>70</v>
       </c>
@@ -1819,13 +1829,13 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.88671875" customWidth="1"/>
-    <col min="2" max="2" width="22.109375" customWidth="1"/>
+    <col min="1" max="1" width="25.85546875" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>116</v>
       </c>
@@ -1833,7 +1843,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>119</v>
       </c>
@@ -1841,7 +1851,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>121</v>
       </c>
@@ -1849,7 +1859,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>123</v>
       </c>
@@ -1857,13 +1867,13 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
     </row>
   </sheetData>
@@ -1879,13 +1889,13 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="5" width="12.5546875" customWidth="1"/>
+    <col min="2" max="5" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -1908,7 +1918,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1916,7 +1926,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1924,12 +1934,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1937,7 +1947,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -1945,7 +1955,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -1956,7 +1966,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>154</v>
       </c>
@@ -1967,7 +1977,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>136</v>
       </c>
@@ -1975,7 +1985,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -1983,7 +1993,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -1991,7 +2001,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -1999,7 +2009,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>136</v>
       </c>
@@ -2010,7 +2020,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>154</v>
       </c>
@@ -2018,7 +2028,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>154</v>
       </c>
@@ -2026,7 +2036,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>154</v>
       </c>
@@ -2034,7 +2044,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>154</v>
       </c>
@@ -2042,7 +2052,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>116</v>
       </c>
@@ -2050,12 +2060,12 @@
         <v>151</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>116</v>
       </c>
@@ -2063,7 +2073,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -2071,7 +2081,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -2079,7 +2089,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -2087,7 +2097,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -2098,7 +2108,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -2106,7 +2116,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -2114,7 +2124,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -2135,9 +2145,9 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -2145,7 +2155,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -2153,12 +2163,12 @@
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>116</v>
       </c>
@@ -2166,7 +2176,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>116</v>
       </c>
@@ -2174,7 +2184,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>116</v>
       </c>
@@ -2182,7 +2192,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>116</v>
       </c>

</xml_diff>